<commit_message>
Updated spreadsheet to include more accurate detailed filter frequency and phase response data
</commit_message>
<xml_diff>
--- a/Documentation/DdD Gain and filter calculations.xlsx
+++ b/Documentation/DdD Gain and filter calculations.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simon\Documents\Personal\Domesday86\Projects\Domesday Duplicator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simon\Documents\GitHub\DomesdayDuplicator\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262D4E6C-9E19-44EE-BCA2-FB6F117AB7CA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10034416-8636-4C31-8F1B-1FD9069E8B14}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8400" windowWidth="38400" windowHeight="19020" xr2:uid="{FBD652DD-93E0-438A-8157-ABC7CFE5D704}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="17610" xr2:uid="{6586ADF8-B05F-4BD6-A150-BEC042DE64BB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Title" sheetId="3" r:id="rId1"/>
-    <sheet name="Gain Setting" sheetId="2" r:id="rId2"/>
-    <sheet name="Filter" sheetId="1" r:id="rId3"/>
+    <sheet name="Gain Setting" sheetId="2" r:id="rId1"/>
+    <sheet name="Filter" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,75 +26,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>mV</t>
+    <t>Hz</t>
   </si>
   <si>
-    <t>Input @ 50R impedance:</t>
+    <t>Log10</t>
   </si>
   <si>
-    <t>mV peak-to-peak</t>
+    <t>Phase</t>
   </si>
   <si>
-    <t>Input signal:</t>
+    <t>1/12 octaves</t>
   </si>
   <si>
-    <t>ohms</t>
+    <t>Amplitude</t>
   </si>
   <si>
-    <t>A</t>
+    <t>Gain (dB)</t>
   </si>
   <si>
-    <t>B</t>
+    <t>mVpp</t>
   </si>
   <si>
-    <t>Note: Must be &gt;200 and &lt; 1500 ohms</t>
+    <t>0 dB level</t>
   </si>
   <si>
-    <t>Parallel resistance:</t>
-  </si>
-  <si>
-    <t>Note: Must be &lt;300 ohms</t>
-  </si>
-  <si>
-    <t>Theoretical gain:</t>
-  </si>
-  <si>
-    <t>Output signal:</t>
-  </si>
-  <si>
-    <t>Output @ 50R impedance:</t>
-  </si>
-  <si>
-    <t>Note: 0 dB point</t>
-  </si>
-  <si>
-    <t>Output @ -3 dB</t>
-  </si>
-  <si>
-    <t>Filter model:</t>
-  </si>
-  <si>
-    <t>Mhz</t>
-  </si>
-  <si>
-    <t>Pass (%)</t>
-  </si>
-  <si>
-    <t>Gain ratio</t>
-  </si>
-  <si>
-    <t>dB</t>
-  </si>
-  <si>
-    <t>Gain settings:</t>
+    <t>DIP switch gain setting calculator:</t>
   </si>
   <si>
     <t>Switch:</t>
-  </si>
-  <si>
-    <t>Ohms:</t>
   </si>
   <si>
     <t>A resistance</t>
@@ -104,51 +64,23 @@
     <t>B resistance</t>
   </si>
   <si>
+    <t>Parallel</t>
+  </si>
+  <si>
     <t>Linear Gain</t>
   </si>
   <si>
     <t>Max input (mV)</t>
   </si>
   <si>
-    <t>DIP switch gain setting calculator:</t>
-  </si>
-  <si>
-    <t>Parallel</t>
-  </si>
-  <si>
-    <t>Filter approximation</t>
-  </si>
-  <si>
-    <t>Domesday Duplicator</t>
-  </si>
-  <si>
-    <t>PCB revision: 2.3</t>
-  </si>
-  <si>
-    <t>© 2018 Simon Inns</t>
-  </si>
-  <si>
-    <t>License: Creative Commons Attribution-ShareAlike 4.0 International (CC BY-SA 4.0)</t>
-  </si>
-  <si>
-    <t>Gain and Filter calculations</t>
-  </si>
-  <si>
-    <t>Note: Filter model is based on pre-production board testing</t>
+    <t>Ohms:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +96,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -171,15 +110,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,29 +125,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
@@ -225,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -248,50 +163,33 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="4"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+  <cellStyles count="4">
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -578,7 +476,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BDFE-4017-BCE5-DD8AFF60ED04}"/>
+              <c16:uniqueId val="{00000000-50E0-4812-A8B5-37A1778997AD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -920,9 +818,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Output (mV)</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Filter frequency</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> response</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -966,11 +869,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Filter!$E$18</c:f>
+              <c:f>Filter!$E$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mV</c:v>
+                  <c:v>Gain (dB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -989,90 +892,264 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Filter!$D$19:$D$30</c:f>
+              <c:f>Filter!$C$6:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>12116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>14678</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>17783</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>21545</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>26102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>31623</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>38312</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>46416</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>56235</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>68130</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>82541</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>121153</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>146780</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>177828</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>215444</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>261016</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>316228</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>383119</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>464159</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>562342</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>681293</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>825405</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1211528</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1467800</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1778280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2154435</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2610158</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3162278</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3831187</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4641589</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5623414</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6812921</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8254042</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12115277</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14677993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17782795</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>21544347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Filter!$E$19:$E$30</c:f>
+              <c:f>Filter!$E$6:$E$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>1890.0768131868133</c:v>
+                  <c:v>-2.3700925320578019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1670.3004395604396</c:v>
+                  <c:v>-1.7142422641316513</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1604.3675274725274</c:v>
+                  <c:v>-1.2031601746838883</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1703.2668956043956</c:v>
+                  <c:v>-0.91034965102608711</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1659.3116208791207</c:v>
+                  <c:v>-0.62708901767979819</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1439.535247252747</c:v>
+                  <c:v>-0.44325380345522664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1736.2333516483516</c:v>
+                  <c:v>-0.26322892115941698</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>241.75401098901096</c:v>
+                  <c:v>-0.17459662517791907</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>109.88818681318681</c:v>
+                  <c:v>-8.6859620215644029E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>153.84346153846153</c:v>
+                  <c:v>-8.6859620215644029E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>153.84346153846153</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>186.8099175824176</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-8.6859620215644029E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-8.6859620215644029E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.17459662517791907</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.26322892115941698</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.35277496825430255</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.44325380345522664</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.62708901767979819</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.91034965102608711</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.2031601746838883</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-1.4039989405667006</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.7142422641316513</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-1.7142422641316513</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.3029990858338694</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.5346850649448941</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.72048658034950108</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.5061870561363073</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-7.7876441007354451</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-32.43909640089803</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-35.960921582011657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1080,7 +1157,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7C2A-4853-BF4A-DDD5386B642D}"/>
+              <c16:uniqueId val="{00000000-63B3-497D-9290-0FE5767BD28C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1092,14 +1169,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2131475679"/>
-        <c:axId val="246394687"/>
+        <c:axId val="1339598912"/>
+        <c:axId val="1617722160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2131475679"/>
+        <c:axId val="1339598912"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="25"/>
+          <c:max val="22000000"/>
+          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1138,8 +1217,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>MHz</a:t>
+                  <a:t>Frequency</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (Hz)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1175,7 +1259,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1209,15 +1293,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246394687"/>
+        <c:crossAx val="1617722160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="246394687"/>
+        <c:axId val="1617722160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1256,7 +1339,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>mV</a:t>
+                  <a:t>Amplitude (dB)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1327,7 +1410,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131475679"/>
+        <c:crossAx val="1339598912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1418,13 +1501,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Output</a:t>
+              <a:t>Filter phase response</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> (dB)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1459,7 +1537,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.9782696709298018E-2"/>
+          <c:y val="8.251558703860902E-2"/>
+          <c:w val="0.86020233979973437"/>
+          <c:h val="0.81042550907902311"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -1468,11 +1556,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Filter!$E$33</c:f>
+              <c:f>Filter!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>dB</c:v>
+                  <c:v>Phase</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1491,90 +1579,261 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Filter!$D$34:$D$45</c:f>
+              <c:f>Filter!$C$6:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>12116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>14678</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>17783</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>21545</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>26102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>31623</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>38312</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>46416</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>56235</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>68130</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>82541</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>121153</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>146780</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>177828</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>215444</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>261016</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>316228</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>383119</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>464159</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>562342</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>681293</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>825405</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1211528</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1467800</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1778280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2154435</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2610158</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3162278</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3831187</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4641589</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5623414</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6812921</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8254042</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12115277</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14677993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17782795</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>21544347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Filter!$E$34:$E$45</c:f>
+              <c:f>Filter!$F$6:$F$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>-0.49085882155051674</c:v>
+                  <c:v>-47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.5645560008060446</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.9143706440127537</c:v>
+                  <c:v>-34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.3947937962956667</c:v>
+                  <c:v>-29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.6218888138381078</c:v>
+                  <c:v>-24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.8560018465862118</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.2282860206130433</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-18.352974143257374</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-25.201427759701499</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-22.278867046136735</c:v>
+                  <c:v>-8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-22.278867046136735</c:v>
+                  <c:v>-7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-20.592449332136017</c:v>
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-170</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-117</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1582,7 +1841,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7419-4895-BA6B-3EF3A3D6ACF8}"/>
+              <c16:uniqueId val="{00000000-0644-4DE4-9085-1C09BFAB8392}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1594,17 +1853,19 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1384655647"/>
-        <c:axId val="1487199871"/>
+        <c:axId val="1338956304"/>
+        <c:axId val="1617716112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1384655647"/>
+        <c:axId val="1338956304"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="25"/>
+          <c:max val="22000000"/>
+          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1622,7 +1883,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1640,11 +1901,19 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>MHz</a:t>
+                  <a:t>Frequency (Hz)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.43859244595566882"/>
+              <c:y val="0.93519675282225412"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1654,7 +1923,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1677,7 +1946,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1711,14 +1980,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1487199871"/>
+        <c:crossAx val="1617716112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1487199871"/>
+        <c:axId val="1617716112"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
+          <c:max val="180"/>
+          <c:min val="-180"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1757,7 +2028,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>dB</a:t>
+                  <a:t>Phase (degrees)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1828,7 +2099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1384655647"/>
+        <c:crossAx val="1338956304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3569,14 +3840,16 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E2B774C-D612-49AB-B450-A36373C3ACE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0061350F-66AC-45F0-96C3-EB5ABD3FFD58}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3597,23 +3870,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="12" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46DF595A-8B74-4C6D-8ABD-268FBD4947E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFCE856-F5C3-4DB1-A5D9-6BC5C6C547ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3633,23 +3906,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="13" name="Chart 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D3FD915-A8C8-4698-8BFC-5F70B30F9F19}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB14326B-31B5-4489-8531-16DA35C85947}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3668,6 +3941,26 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96140FBA-480D-4BF6-B0B9-5F38600184F9}" name="Table2" displayName="Table2" ref="B5:F46" totalsRowShown="0">
+  <autoFilter ref="B5:F46" xr:uid="{350EAA1F-12FF-4FCD-B71B-F94E77BA9594}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A70284C1-E80D-4A48-AFFC-1809B06CFC86}" name="Log10">
+      <calculatedColumnFormula>B5 + (1/12)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{DC4E205A-4452-4215-B462-9FA2CDDDD201}" name="Hz">
+      <calculatedColumnFormula xml:space="preserve"> ROUNDUP(10 ^ B6, 0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{3C366408-4A01-4F38-87AA-2A3C31477FD3}" name="Amplitude"/>
+    <tableColumn id="4" xr3:uid="{9B7FDE06-47E8-4787-B4F9-EE412CAFE2F9}" name="Gain (dB)" dataDxfId="0">
+      <calculatedColumnFormula>20*LOG10(D6 / $D$2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{268775CA-9D02-490D-8233-D0A8E7F2DE25}" name="Phase"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3966,49 +4259,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B1FFA3-BA2B-4B48-8420-45B6ADA3BFEA}">
-  <dimension ref="B2:B8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3D897B-3613-45D6-BDBA-AE034B428C1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5473A75-8EE1-4908-A621-0E8DCAAAB26F}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4019,70 +4274,70 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>4</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>2</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
         <v>3</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="M4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="N4" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="R4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="7">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3">
         <v>1500</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="3">
         <v>1000</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="3">
         <v>680</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="3">
         <v>560</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="3">
         <v>200</v>
       </c>
     </row>
@@ -4090,57 +4345,57 @@
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="9">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9">
-        <f>IF(B7 = 1, 1 / B$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="9">
-        <f>IF(C7 = 1, 1 / C$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
-        <f>IF(D7 = 1, 1 / D$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
-        <f>IF(E7 = 1, 1 / E$5, 0)</f>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4">
+        <f t="shared" ref="G7:J21" si="0">IF(B7 = 1, 1 / B$5, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="0"/>
         <v>1.7857142857142857E-3</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
         <f>1 / SUM(G7:J7)</f>
         <v>560</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="4">
         <f>$M$5</f>
         <v>200</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="4">
         <f>(L7*M7)/(L7+M7)</f>
         <v>147.36842105263159</v>
       </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="8">
-        <f t="shared" ref="P7:P21" si="0">ROUND(1 + (L7 / M7),2)</f>
+      <c r="O7" s="4"/>
+      <c r="P7" s="5">
+        <f t="shared" ref="P7:P21" si="1">ROUND(1 + (L7 / M7),2)</f>
         <v>3.8</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="4">
         <v>1</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="6">
         <f>2000 / P7</f>
         <v>526.31578947368428</v>
       </c>
@@ -4162,42 +4417,42 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>IF(B8 = 1, 1 / B$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>IF(C8 = 1, 1 / C$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f>IF(D8 = 1, 1 / D$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>1.4705882352941176E-3</v>
       </c>
       <c r="J8">
-        <f>IF(E8 = 1, 1 / E$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L8">
-        <f t="shared" ref="L8:L21" si="1">1 / SUM(G8:J8)</f>
+        <f t="shared" ref="L8:L21" si="2">1 / SUM(G8:J8)</f>
         <v>680</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:M21" si="2">$M$5</f>
+        <f t="shared" ref="M8:M21" si="3">$M$5</f>
         <v>200</v>
       </c>
       <c r="N8">
-        <f t="shared" ref="N8:N21" si="3">(L8*M8)/(L8+M8)</f>
+        <f t="shared" ref="N8:N21" si="4">(L8*M8)/(L8+M8)</f>
         <v>154.54545454545453</v>
       </c>
-      <c r="P8" s="8">
-        <f t="shared" si="0"/>
+      <c r="P8" s="5">
+        <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="Q8">
         <v>2</v>
       </c>
-      <c r="R8" s="6">
-        <f t="shared" ref="R8:R21" si="4">2000 / P8</f>
+      <c r="R8" s="1">
+        <f t="shared" ref="R8:R21" si="5">2000 / P8</f>
         <v>454.5454545454545</v>
       </c>
     </row>
@@ -4205,58 +4460,58 @@
       <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9" s="9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9">
-        <f>IF(B9 = 1, 1 / B$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <f>IF(C9 = 1, 1 / C$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
-        <f>IF(D9 = 1, 1 / D$5, 0)</f>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
         <v>1.4705882352941176E-3</v>
       </c>
-      <c r="J9" s="9">
-        <f>IF(E9 = 1, 1 / E$5, 0)</f>
+      <c r="J9" s="4">
+        <f t="shared" si="0"/>
         <v>1.7857142857142857E-3</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
+        <f t="shared" si="2"/>
+        <v>307.09677419354841</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="4"/>
+        <v>121.11959287531806</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="5">
         <f t="shared" si="1"/>
-        <v>307.09677419354841</v>
-      </c>
-      <c r="M9" s="9">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N9" s="9">
-        <f t="shared" si="3"/>
-        <v>121.11959287531806</v>
-      </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="8">
-        <f t="shared" si="0"/>
         <v>2.54</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="4">
         <v>3</v>
       </c>
-      <c r="R9" s="10">
-        <f t="shared" si="4"/>
+      <c r="R9" s="6">
+        <f t="shared" si="5"/>
         <v>787.40157480314963</v>
       </c>
     </row>
@@ -4277,42 +4532,42 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>IF(B10 = 1, 1 / B$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>IF(C10 = 1, 1 / C$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="I10">
-        <f>IF(D10 = 1, 1 / D$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>IF(E10 = 1, 1 / E$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L10">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="P10" s="5">
         <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="3"/>
-        <v>166.66666666666666</v>
-      </c>
-      <c r="P10" s="8">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="Q10">
         <v>4</v>
       </c>
-      <c r="R10" s="6">
-        <f t="shared" si="4"/>
+      <c r="R10" s="1">
+        <f t="shared" si="5"/>
         <v>333.33333333333331</v>
       </c>
     </row>
@@ -4320,58 +4575,58 @@
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9">
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
         <v>1</v>
       </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9">
-        <f>IF(B11 = 1, 1 / B$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="9">
-        <f>IF(C11 = 1, 1 / C$5, 0)</f>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="I11" s="9">
-        <f>IF(D11 = 1, 1 / D$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="9">
-        <f>IF(E11 = 1, 1 / E$5, 0)</f>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" si="0"/>
         <v>1.7857142857142857E-3</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
+        <f t="shared" si="2"/>
+        <v>358.97435897435901</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="4"/>
+        <v>128.44036697247705</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="5">
         <f t="shared" si="1"/>
-        <v>358.97435897435901</v>
-      </c>
-      <c r="M11" s="9">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N11" s="9">
-        <f t="shared" si="3"/>
-        <v>128.44036697247705</v>
-      </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="8">
-        <f t="shared" si="0"/>
         <v>2.79</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="Q11" s="4">
         <v>5</v>
       </c>
-      <c r="R11" s="10">
-        <f t="shared" si="4"/>
+      <c r="R11" s="6">
+        <f t="shared" si="5"/>
         <v>716.84587813620067</v>
       </c>
     </row>
@@ -4392,42 +4647,42 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <f>IF(B12 = 1, 1 / B$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f>IF(C12 = 1, 1 / C$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="I12">
-        <f>IF(D12 = 1, 1 / D$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>1.4705882352941176E-3</v>
       </c>
       <c r="J12">
-        <f>IF(E12 = 1, 1 / E$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L12">
+        <f t="shared" si="2"/>
+        <v>404.76190476190476</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>133.85826771653541</v>
+      </c>
+      <c r="P12" s="5">
         <f t="shared" si="1"/>
-        <v>404.76190476190476</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="3"/>
-        <v>133.85826771653541</v>
-      </c>
-      <c r="P12" s="8">
-        <f t="shared" si="0"/>
         <v>3.02</v>
       </c>
       <c r="Q12">
         <v>6</v>
       </c>
-      <c r="R12" s="6">
-        <f t="shared" si="4"/>
+      <c r="R12" s="1">
+        <f t="shared" si="5"/>
         <v>662.25165562913912</v>
       </c>
     </row>
@@ -4435,58 +4690,58 @@
       <c r="A13">
         <v>7</v>
       </c>
-      <c r="B13" s="9">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9">
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
         <v>1</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="4">
         <v>1</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="4">
         <v>1</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9">
-        <f>IF(B13 = 1, 1 / B$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="9">
-        <f>IF(C13 = 1, 1 / C$5, 0)</f>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="I13" s="9">
-        <f>IF(D13 = 1, 1 / D$5, 0)</f>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
         <v>1.4705882352941176E-3</v>
       </c>
-      <c r="J13" s="9">
-        <f>IF(E13 = 1, 1 / E$5, 0)</f>
+      <c r="J13" s="4">
+        <f t="shared" si="0"/>
         <v>1.7857142857142857E-3</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4">
+        <f t="shared" si="2"/>
+        <v>234.94570582428432</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="4"/>
+        <v>108.03449841125736</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="5">
         <f t="shared" si="1"/>
-        <v>234.94570582428432</v>
-      </c>
-      <c r="M13" s="9">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N13" s="9">
-        <f t="shared" si="3"/>
-        <v>108.03449841125736</v>
-      </c>
-      <c r="O13" s="9"/>
-      <c r="P13" s="8">
-        <f t="shared" si="0"/>
         <v>2.17</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="4">
         <v>7</v>
       </c>
-      <c r="R13" s="10">
-        <f t="shared" si="4"/>
+      <c r="R13" s="6">
+        <f t="shared" si="5"/>
         <v>921.65898617511527</v>
       </c>
     </row>
@@ -4507,42 +4762,42 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f>IF(B14 = 1, 1 / B$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>6.6666666666666664E-4</v>
       </c>
       <c r="H14">
-        <f>IF(C14 = 1, 1 / C$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>IF(D14 = 1, 1 / D$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14">
-        <f>IF(E14 = 1, 1 / E$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L14">
+        <f t="shared" si="2"/>
+        <v>1500</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>176.47058823529412</v>
+      </c>
+      <c r="P14" s="5">
         <f t="shared" si="1"/>
-        <v>1500</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="3"/>
-        <v>176.47058823529412</v>
-      </c>
-      <c r="P14" s="8">
-        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="Q14">
         <v>8</v>
       </c>
-      <c r="R14" s="6">
-        <f t="shared" si="4"/>
+      <c r="R14" s="1">
+        <f t="shared" si="5"/>
         <v>235.29411764705881</v>
       </c>
     </row>
@@ -4550,58 +4805,58 @@
       <c r="A15">
         <v>9</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="9">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
         <v>1</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9">
-        <f>IF(B15 = 1, 1 / B$5, 0)</f>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
         <v>6.6666666666666664E-4</v>
       </c>
-      <c r="H15" s="9">
-        <f>IF(C15 = 1, 1 / C$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="9">
-        <f>IF(D15 = 1, 1 / D$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="9">
-        <f>IF(E15 = 1, 1 / E$5, 0)</f>
+      <c r="H15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="0"/>
         <v>1.7857142857142857E-3</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9">
+      <c r="K15" s="4"/>
+      <c r="L15" s="4">
+        <f t="shared" si="2"/>
+        <v>407.76699029126212</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" si="4"/>
+        <v>134.18530351437698</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="5">
         <f t="shared" si="1"/>
-        <v>407.76699029126212</v>
-      </c>
-      <c r="M15" s="9">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N15" s="9">
-        <f t="shared" si="3"/>
-        <v>134.18530351437698</v>
-      </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="8">
-        <f t="shared" si="0"/>
         <v>3.04</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="Q15" s="4">
         <v>9</v>
       </c>
-      <c r="R15" s="10">
-        <f t="shared" si="4"/>
+      <c r="R15" s="6">
+        <f t="shared" si="5"/>
         <v>657.8947368421052</v>
       </c>
     </row>
@@ -4622,42 +4877,42 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f>IF(B16 = 1, 1 / B$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>6.6666666666666664E-4</v>
       </c>
       <c r="H16">
-        <f>IF(C16 = 1, 1 / C$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>IF(D16 = 1, 1 / D$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>1.4705882352941176E-3</v>
       </c>
       <c r="J16">
-        <f>IF(E16 = 1, 1 / E$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L16">
+        <f t="shared" si="2"/>
+        <v>467.88990825688074</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>140.1098901098901</v>
+      </c>
+      <c r="P16" s="5">
         <f t="shared" si="1"/>
-        <v>467.88990825688074</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="3"/>
-        <v>140.1098901098901</v>
-      </c>
-      <c r="P16" s="8">
-        <f t="shared" si="0"/>
         <v>3.34</v>
       </c>
       <c r="Q16">
         <v>10</v>
       </c>
-      <c r="R16" s="6">
-        <f t="shared" si="4"/>
+      <c r="R16" s="1">
+        <f t="shared" si="5"/>
         <v>598.80239520958082</v>
       </c>
     </row>
@@ -4665,58 +4920,58 @@
       <c r="A17">
         <v>11</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="4">
         <v>1</v>
       </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
         <v>1</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="4">
         <v>1</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9">
-        <f>IF(B17 = 1, 1 / B$5, 0)</f>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
         <v>6.6666666666666664E-4</v>
       </c>
-      <c r="H17" s="9">
-        <f>IF(C17 = 1, 1 / C$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
-        <f>IF(D17 = 1, 1 / D$5, 0)</f>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="0"/>
         <v>1.4705882352941176E-3</v>
       </c>
-      <c r="J17" s="9">
-        <f>IF(E17 = 1, 1 / E$5, 0)</f>
+      <c r="J17" s="4">
+        <f t="shared" si="0"/>
         <v>1.7857142857142857E-3</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4">
+        <f t="shared" si="2"/>
+        <v>254.90896108532667</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" si="4"/>
+        <v>112.07031863129806</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="5">
         <f t="shared" si="1"/>
-        <v>254.90896108532667</v>
-      </c>
-      <c r="M17" s="9">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N17" s="9">
-        <f t="shared" si="3"/>
-        <v>112.07031863129806</v>
-      </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="8">
-        <f t="shared" si="0"/>
         <v>2.27</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="Q17" s="4">
         <v>11</v>
       </c>
-      <c r="R17" s="10">
-        <f t="shared" si="4"/>
+      <c r="R17" s="6">
+        <f t="shared" si="5"/>
         <v>881.05726872246692</v>
       </c>
     </row>
@@ -4737,42 +4992,42 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <f>IF(B18 = 1, 1 / B$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>6.6666666666666664E-4</v>
       </c>
       <c r="H18">
-        <f>IF(C18 = 1, 1 / C$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="I18">
-        <f>IF(D18 = 1, 1 / D$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J18">
-        <f>IF(E18 = 1, 1 / E$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L18">
+        <f t="shared" si="2"/>
+        <v>600</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="P18" s="5">
         <f t="shared" si="1"/>
-        <v>600</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="3"/>
-        <v>150</v>
-      </c>
-      <c r="P18" s="8">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="Q18">
         <v>12</v>
       </c>
-      <c r="R18" s="6">
-        <f t="shared" si="4"/>
+      <c r="R18" s="1">
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
     </row>
@@ -4780,58 +5035,58 @@
       <c r="A19">
         <v>13</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="4">
         <v>1</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-      <c r="E19" s="9">
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
         <v>1</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9">
-        <f>IF(B19 = 1, 1 / B$5, 0)</f>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
         <v>6.6666666666666664E-4</v>
       </c>
-      <c r="H19" s="9">
-        <f>IF(C19 = 1, 1 / C$5, 0)</f>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="I19" s="9">
-        <f>IF(D19 = 1, 1 / D$5, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="9">
-        <f>IF(E19 = 1, 1 / E$5, 0)</f>
+      <c r="I19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="0"/>
         <v>1.7857142857142857E-3</v>
       </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9">
+      <c r="K19" s="4"/>
+      <c r="L19" s="4">
+        <f t="shared" si="2"/>
+        <v>289.65517241379308</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" si="4"/>
+        <v>118.30985915492957</v>
+      </c>
+      <c r="O19" s="4"/>
+      <c r="P19" s="5">
         <f t="shared" si="1"/>
-        <v>289.65517241379308</v>
-      </c>
-      <c r="M19" s="9">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N19" s="9">
-        <f t="shared" si="3"/>
-        <v>118.30985915492957</v>
-      </c>
-      <c r="O19" s="9"/>
-      <c r="P19" s="8">
-        <f t="shared" si="0"/>
         <v>2.4500000000000002</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="Q19" s="4">
         <v>13</v>
       </c>
-      <c r="R19" s="10">
-        <f t="shared" si="4"/>
+      <c r="R19" s="6">
+        <f t="shared" si="5"/>
         <v>816.32653061224482</v>
       </c>
     </row>
@@ -4852,42 +5107,42 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <f>IF(B20 = 1, 1 / B$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>6.6666666666666664E-4</v>
       </c>
       <c r="H20">
-        <f>IF(C20 = 1, 1 / C$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="I20">
-        <f>IF(D20 = 1, 1 / D$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>1.4705882352941176E-3</v>
       </c>
       <c r="J20">
-        <f>IF(E20 = 1, 1 / E$5, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L20">
+        <f t="shared" si="2"/>
+        <v>318.75</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>122.89156626506023</v>
+      </c>
+      <c r="P20" s="5">
         <f t="shared" si="1"/>
-        <v>318.75</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="3"/>
-        <v>122.89156626506023</v>
-      </c>
-      <c r="P20" s="8">
-        <f t="shared" si="0"/>
         <v>2.59</v>
       </c>
       <c r="Q20">
         <v>14</v>
       </c>
-      <c r="R20" s="6">
-        <f t="shared" si="4"/>
+      <c r="R20" s="1">
+        <f t="shared" si="5"/>
         <v>772.20077220077224</v>
       </c>
     </row>
@@ -4895,517 +5150,963 @@
       <c r="A21">
         <v>15</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="4">
         <v>1</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="4">
         <v>1</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="4">
         <v>1</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9">
-        <f>IF(B21 = 1, 1 / B$5, 0)</f>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
         <v>6.6666666666666664E-4</v>
       </c>
-      <c r="H21" s="9">
-        <f>IF(C21 = 1, 1 / C$5, 0)</f>
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="I21" s="9">
-        <f>IF(D21 = 1, 1 / D$5, 0)</f>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
         <v>1.4705882352941176E-3</v>
       </c>
-      <c r="J21" s="9">
-        <f>IF(E21 = 1, 1 / E$5, 0)</f>
+      <c r="J21" s="4">
+        <f t="shared" si="0"/>
         <v>1.7857142857142857E-3</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9">
+      <c r="K21" s="4"/>
+      <c r="L21" s="4">
+        <f t="shared" si="2"/>
+        <v>203.12944523470838</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="4"/>
+        <v>100.77628793225124</v>
+      </c>
+      <c r="O21" s="4"/>
+      <c r="P21" s="5">
         <f t="shared" si="1"/>
-        <v>203.12944523470838</v>
-      </c>
-      <c r="M21" s="9">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="N21" s="9">
-        <f t="shared" si="3"/>
-        <v>100.77628793225124</v>
-      </c>
-      <c r="O21" s="9"/>
-      <c r="P21" s="8">
-        <f t="shared" si="0"/>
         <v>2.02</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="Q21" s="4">
         <v>15</v>
       </c>
-      <c r="R21" s="10">
-        <f t="shared" si="4"/>
+      <c r="R21" s="6">
+        <f t="shared" si="5"/>
         <v>990.09900990099004</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F609BA2-22D8-4AEF-8316-23966852B572}">
-  <dimension ref="A1:G49"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>235.29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>1500</v>
-      </c>
-      <c r="D7">
-        <v>200</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5">
-        <f>(C7*D7)/(C7+D7)</f>
-        <v>176.47058823529412</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2">
-        <f>1+(C7/D7)</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2">
-        <f>C4 * C11</f>
-        <v>1999.9649999999999</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <f>C14 * SQRT(2)/2</f>
-        <v>1414.1888136357536</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="3">
-        <v>94.505494505494511</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" ref="E19:E30" si="0">($C$14 / 100) * C19</f>
-        <v>1890.0768131868133</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="3">
-        <v>83.516483516483518</v>
-      </c>
-      <c r="D20" s="3">
-        <v>4</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="0"/>
-        <v>1670.3004395604396</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="3">
-        <v>80.219780219780219</v>
-      </c>
-      <c r="D21" s="3">
-        <v>6</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="0"/>
-        <v>1604.3675274725274</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="3">
-        <v>85.164835164835168</v>
-      </c>
-      <c r="D22" s="3">
-        <v>8</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="0"/>
-        <v>1703.2668956043956</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="3">
-        <v>82.967032967032964</v>
-      </c>
-      <c r="D23" s="3">
-        <v>10</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="0"/>
-        <v>1659.3116208791207</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="3">
-        <v>71.978021978021971</v>
-      </c>
-      <c r="D24" s="3">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="0"/>
-        <v>1439.535247252747</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="3">
-        <v>86.813186813186817</v>
-      </c>
-      <c r="D25" s="3">
-        <v>14</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="shared" si="0"/>
-        <v>1736.2333516483516</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="4">
-        <v>12.087912087912088</v>
-      </c>
-      <c r="D26" s="4">
-        <v>16</v>
-      </c>
-      <c r="E26" s="4">
-        <f t="shared" si="0"/>
-        <v>241.75401098901096</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="4">
-        <v>5.4945054945054945</v>
-      </c>
-      <c r="D27" s="4">
-        <v>18</v>
-      </c>
-      <c r="E27" s="4">
-        <f t="shared" si="0"/>
-        <v>109.88818681318681</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="4">
-        <v>7.6923076923076925</v>
-      </c>
-      <c r="D28" s="4">
-        <v>20</v>
-      </c>
-      <c r="E28" s="4">
-        <f t="shared" si="0"/>
-        <v>153.84346153846153</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="4">
-        <v>7.6923076923076925</v>
-      </c>
-      <c r="D29" s="4">
-        <v>22</v>
-      </c>
-      <c r="E29" s="4">
-        <f t="shared" si="0"/>
-        <v>153.84346153846153</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="4">
-        <v>9.3406593406593412</v>
-      </c>
-      <c r="D30" s="4">
-        <v>24</v>
-      </c>
-      <c r="E30" s="4">
-        <f t="shared" si="0"/>
-        <v>186.8099175824176</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="3">
-        <f t="shared" ref="C34:C45" si="1">E19 / $C$14</f>
-        <v>0.94505494505494514</v>
-      </c>
-      <c r="D34" s="3">
-        <v>2</v>
-      </c>
-      <c r="E34" s="3">
-        <f t="shared" ref="E34:E45" si="2">20 *LOG10(C34)</f>
-        <v>-0.49085882155051674</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="3">
-        <f t="shared" si="1"/>
-        <v>0.8351648351648352</v>
-      </c>
-      <c r="D35" s="3">
-        <v>4</v>
-      </c>
-      <c r="E35" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.5645560008060446</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="3">
-        <f t="shared" si="1"/>
-        <v>0.80219780219780223</v>
-      </c>
-      <c r="D36" s="3">
-        <v>6</v>
-      </c>
-      <c r="E36" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.9143706440127537</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="3">
-        <f t="shared" si="1"/>
-        <v>0.85164835164835162</v>
-      </c>
-      <c r="D37" s="3">
-        <v>8</v>
-      </c>
-      <c r="E37" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.3947937962956667</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="3">
-        <f t="shared" si="1"/>
-        <v>0.82967032967032961</v>
-      </c>
-      <c r="D38" s="3">
-        <v>10</v>
-      </c>
-      <c r="E38" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.6218888138381078</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="3">
-        <f t="shared" si="1"/>
-        <v>0.71978021978021967</v>
-      </c>
-      <c r="D39" s="3">
-        <v>12</v>
-      </c>
-      <c r="E39" s="3">
-        <f t="shared" si="2"/>
-        <v>-2.8560018465862118</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="3">
-        <f t="shared" si="1"/>
-        <v>0.86813186813186816</v>
-      </c>
-      <c r="D40" s="3">
-        <v>14</v>
-      </c>
-      <c r="E40" s="3">
-        <f t="shared" si="2"/>
-        <v>-1.2282860206130433</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="4">
-        <f t="shared" si="1"/>
-        <v>0.12087912087912087</v>
-      </c>
-      <c r="D41" s="4">
-        <v>16</v>
-      </c>
-      <c r="E41" s="4">
-        <f t="shared" si="2"/>
-        <v>-18.352974143257374</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="4">
-        <f t="shared" si="1"/>
-        <v>5.4945054945054944E-2</v>
-      </c>
-      <c r="D42" s="4">
-        <v>18</v>
-      </c>
-      <c r="E42" s="4">
-        <f t="shared" si="2"/>
-        <v>-25.201427759701499</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="4">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076913E-2</v>
-      </c>
-      <c r="D43" s="4">
-        <v>20</v>
-      </c>
-      <c r="E43" s="4">
-        <f t="shared" si="2"/>
-        <v>-22.278867046136735</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="4">
-        <f t="shared" si="1"/>
-        <v>7.6923076923076913E-2</v>
-      </c>
-      <c r="D44" s="4">
-        <v>22</v>
-      </c>
-      <c r="E44" s="4">
-        <f t="shared" si="2"/>
-        <v>-22.278867046136735</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="4">
-        <f t="shared" si="1"/>
-        <v>9.3406593406593422E-2</v>
-      </c>
-      <c r="D45" s="4">
-        <v>24</v>
-      </c>
-      <c r="E45" s="4">
-        <f t="shared" si="2"/>
-        <v>-20.592449332136017</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696FC061-23D0-40B8-BFCA-2B0991513C23}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:K46"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2010</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B6, 0)</f>
+        <v>10000</v>
+      </c>
+      <c r="D6">
+        <v>1530</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E46" si="0">20*LOG10(D6 / $D$2)</f>
+        <v>-2.3700925320578019</v>
+      </c>
+      <c r="F6">
+        <v>-47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" ref="B6:B12" si="1">B6 + (1/12)</f>
+        <v>4.083333333333333</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C60" si="2" xml:space="preserve"> ROUNDUP(10 ^ B7, 0)</f>
+        <v>12116</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1650</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>-1.7142422641316513</v>
+      </c>
+      <c r="F7">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>4.1666666666666661</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>14678</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1750</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-1.2031601746838883</v>
+      </c>
+      <c r="F8">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>4.2499999999999991</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>17783</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1810</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-0.91034965102608711</v>
+      </c>
+      <c r="F9">
+        <v>-29</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>4.3333333333333321</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>21545</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1870</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-0.62708901767979819</v>
+      </c>
+      <c r="F10">
+        <v>-24</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>4.4166666666666652</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>26102</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1910</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-0.44325380345522664</v>
+      </c>
+      <c r="F11">
+        <v>-20</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>4.4999999999999982</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>31623</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1950</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>-0.26322892115941698</v>
+      </c>
+      <c r="F12">
+        <v>-16</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>B12 + (1/12)</f>
+        <v>4.5833333333333313</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>38312</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1970</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-0.17459662517791907</v>
+      </c>
+      <c r="F13">
+        <v>-13</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" ref="B14:B26" si="3">B13 + (1/12)</f>
+        <v>4.6666666666666643</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>46416</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1990</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-8.6859620215644029E-2</v>
+      </c>
+      <c r="F14">
+        <v>-10</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="3"/>
+        <v>4.7499999999999973</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>56235</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1990</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>-8.6859620215644029E-2</v>
+      </c>
+      <c r="F15">
+        <v>-8</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" si="3"/>
+        <v>4.8333333333333304</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>68130</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>-7</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" si="3"/>
+        <v>4.9166666666666634</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>82541</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>-5</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" si="3"/>
+        <v>4.9999999999999964</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>100000</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>-4</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="3"/>
+        <v>5.0833333333333295</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>121153</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>-2</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="3"/>
+        <v>5.1666666666666625</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>146780</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="3"/>
+        <v>5.2499999999999956</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>177828</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f t="shared" si="3"/>
+        <v>5.3333333333333286</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>215444</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f t="shared" si="3"/>
+        <v>5.4166666666666616</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>261016</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" si="3"/>
+        <v>5.4999999999999947</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>316228</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f t="shared" si="3"/>
+        <v>5.5833333333333277</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>383119</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f t="shared" si="3"/>
+        <v>5.6666666666666607</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>464159</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>B26 + (1/12)</f>
+        <v>5.7499999999999938</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>562342</v>
+      </c>
+      <c r="D27">
+        <v>2010</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>11</v>
+      </c>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" ref="B28:B46" si="4">B27 + (1/12)</f>
+        <v>5.8333333333333268</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>681293</v>
+      </c>
+      <c r="D28">
+        <v>1990</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>-8.6859620215644029E-2</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f t="shared" si="4"/>
+        <v>5.9166666666666599</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>825405</v>
+      </c>
+      <c r="D29">
+        <v>1990</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>-8.6859620215644029E-2</v>
+      </c>
+      <c r="F29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f t="shared" si="4"/>
+        <v>5.9999999999999929</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>1000000</v>
+      </c>
+      <c r="D30">
+        <v>1970</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>-0.17459662517791907</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" si="4"/>
+        <v>6.0833333333333259</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>1211528</v>
+      </c>
+      <c r="D31">
+        <v>1950</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>-0.26322892115941698</v>
+      </c>
+      <c r="F31">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f t="shared" si="4"/>
+        <v>6.166666666666659</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>1467800</v>
+      </c>
+      <c r="D32">
+        <v>1930</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>-0.35277496825430255</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f t="shared" si="4"/>
+        <v>6.249999999999992</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>1778280</v>
+      </c>
+      <c r="D33">
+        <v>1910</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>-0.44325380345522664</v>
+      </c>
+      <c r="F33">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f t="shared" si="4"/>
+        <v>6.333333333333325</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>2154435</v>
+      </c>
+      <c r="D34">
+        <v>1870</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>-0.62708901767979819</v>
+      </c>
+      <c r="F34">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" si="4"/>
+        <v>6.4166666666666581</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>2610158</v>
+      </c>
+      <c r="D35">
+        <v>1810</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>-0.91034965102608711</v>
+      </c>
+      <c r="F35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" si="4"/>
+        <v>6.4999999999999911</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>3162278</v>
+      </c>
+      <c r="D36">
+        <v>1750</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>-1.2031601746838883</v>
+      </c>
+      <c r="F36">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" si="4"/>
+        <v>6.5833333333333242</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>3831187</v>
+      </c>
+      <c r="D37">
+        <v>1710</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>-1.4039989405667006</v>
+      </c>
+      <c r="F37">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" si="4"/>
+        <v>6.6666666666666572</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>4641589</v>
+      </c>
+      <c r="D38">
+        <v>1650</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>-1.7142422641316513</v>
+      </c>
+      <c r="F38">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" si="4"/>
+        <v>6.7499999999999902</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>5623414</v>
+      </c>
+      <c r="D39">
+        <v>1650</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>-1.7142422641316513</v>
+      </c>
+      <c r="F39">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" si="4"/>
+        <v>6.8333333333333233</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>6812921</v>
+      </c>
+      <c r="D40">
+        <v>1730</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>-1.3029990858338694</v>
+      </c>
+      <c r="F40">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" si="4"/>
+        <v>6.9166666666666563</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>8254042</v>
+      </c>
+      <c r="D41">
+        <v>1890</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>-0.5346850649448941</v>
+      </c>
+      <c r="F41">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f t="shared" si="4"/>
+        <v>6.9999999999999893</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>10000000</v>
+      </c>
+      <c r="D42">
+        <v>1850</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>-0.72048658034950108</v>
+      </c>
+      <c r="F42">
+        <v>-170</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f t="shared" si="4"/>
+        <v>7.0833333333333224</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>12115277</v>
+      </c>
+      <c r="D43">
+        <v>1690</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>-1.5061870561363073</v>
+      </c>
+      <c r="F43">
+        <v>-117</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <f t="shared" si="4"/>
+        <v>7.1666666666666554</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>14677993</v>
+      </c>
+      <c r="D44">
+        <v>820</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>-7.7876441007354451</v>
+      </c>
+      <c r="F44">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <f t="shared" si="4"/>
+        <v>7.2499999999999885</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>17782795</v>
+      </c>
+      <c r="D45">
+        <v>48</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>-32.43909640089803</v>
+      </c>
+      <c r="F45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f t="shared" si="4"/>
+        <v>7.3333333333333215</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>21544347</v>
+      </c>
+      <c r="D46">
+        <v>32</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>-35.960921582011657</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated frequency response documentation
</commit_message>
<xml_diff>
--- a/Documentation/DdD Gain and filter calculations.xlsx
+++ b/Documentation/DdD Gain and filter calculations.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simon\Documents\GitHub\DomesdayDuplicator\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10034416-8636-4C31-8F1B-1FD9069E8B14}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4482452F-43C9-4709-BD12-325460353449}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="17610" xr2:uid="{6586ADF8-B05F-4BD6-A150-BEC042DE64BB}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="38400" windowHeight="17610" activeTab="1" xr2:uid="{6586ADF8-B05F-4BD6-A150-BEC042DE64BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gain Setting" sheetId="2" r:id="rId1"/>
-    <sheet name="Filter" sheetId="1" r:id="rId2"/>
+    <sheet name="ADC output response" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,30 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Hz</t>
   </si>
   <si>
     <t>Log10</t>
-  </si>
-  <si>
-    <t>Phase</t>
-  </si>
-  <si>
-    <t>1/12 octaves</t>
-  </si>
-  <si>
-    <t>Amplitude</t>
-  </si>
-  <si>
-    <t>Gain (dB)</t>
-  </si>
-  <si>
-    <t>mVpp</t>
-  </si>
-  <si>
-    <t>0 dB level</t>
   </si>
   <si>
     <t>DIP switch gain setting calculator:</t>
@@ -75,11 +57,32 @@
   <si>
     <t>Ohms:</t>
   </si>
+  <si>
+    <t>Peak</t>
+  </si>
+  <si>
+    <t>RMS peak</t>
+  </si>
+  <si>
+    <t>200mVPP input with gain switch 1000</t>
+  </si>
+  <si>
+    <t>Peak dB</t>
+  </si>
+  <si>
+    <t>RMS Peak dB</t>
+  </si>
+  <si>
+    <t>Note: 0dB is relative to ADC maximum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,7 +173,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -178,6 +181,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -185,11 +190,7 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -799,36 +800,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Filter frequency</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> response</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -869,11 +840,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Filter!$E$5</c:f>
+              <c:f>'ADC output response'!$E$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gain (dB)</c:v>
+                  <c:v>Peak dB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -892,9 +863,9 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Filter!$C$6:$C$46</c:f>
+              <c:f>'ADC output response'!$D$6:$D$46</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>10000</c:v>
@@ -1024,132 +995,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Filter!$E$6:$E$46</c:f>
+              <c:f>'ADC output response'!$E$6:$E$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>-2.3700925320578019</c:v>
+                  <c:v>-3.9569408226557687</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.7142422641316513</c:v>
+                  <c:v>-3.216889871943414</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.2031601746838883</c:v>
+                  <c:v>-2.6692558380816345</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.91034965102608711</c:v>
+                  <c:v>-2.2637580608355079</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.62708901767979819</c:v>
+                  <c:v>-1.9809312005754807</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.44325380345522664</c:v>
+                  <c:v>-1.7481837792480062</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.26322892115941698</c:v>
+                  <c:v>-1.6038936228528302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.17459662517791907</c:v>
+                  <c:v>-1.5024380793839742</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-8.6859620215644029E-2</c:v>
+                  <c:v>-1.4222452027494425</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-8.6859620215644029E-2</c:v>
+                  <c:v>-1.3891388258243724</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-1.3487998762784796</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>-1.3290293962371769</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>-1.3231403965924835</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>-1.3096976857579279</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-1.3093543100847316</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>-1.3036703854417109</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>-1.3035290918940998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>-1.3037208479800224</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>-1.3090210466770615</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>-1.3238484843225506</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>-1.3288573241619814</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>-1.3437288305971651</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-8.6859620215644029E-2</c:v>
+                  <c:v>-1.3680765606671534</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-8.6859620215644029E-2</c:v>
+                  <c:v>-1.4233093127111565</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.17459662517791907</c:v>
+                  <c:v>-1.4675646675716463</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.26322892115941698</c:v>
+                  <c:v>-1.5653551394136862</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.35277496825430255</c:v>
+                  <c:v>-1.6677841468865393</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.44325380345522664</c:v>
+                  <c:v>-1.8342359728863094</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.62708901767979819</c:v>
+                  <c:v>-2.0469414341029211</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.91034965102608711</c:v>
+                  <c:v>-2.3293377035635094</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-1.2031601746838883</c:v>
+                  <c:v>-2.6237151138378687</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-1.4039989405667006</c:v>
+                  <c:v>-2.9746617562437736</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-1.7142422641316513</c:v>
+                  <c:v>-3.2668855156566847</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-1.7142422641316513</c:v>
+                  <c:v>-3.3406935865431637</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-1.3029990858338694</c:v>
+                  <c:v>-3.0944291016408734</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.5346850649448941</c:v>
+                  <c:v>-2.6229632118397062</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.72048658034950108</c:v>
+                  <c:v>-3.0480039660192979</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-1.5061870561363073</c:v>
+                  <c:v>-4.7399954493073375</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-7.7876441007354451</c:v>
+                  <c:v>-4.0375159626601489</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-32.43909640089803</c:v>
+                  <c:v>-29.729522077725093</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-35.960921582011657</c:v>
+                  <c:v>-43.521390897488729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1157,7 +1128,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-63B3-497D-9290-0FE5767BD28C}"/>
+              <c16:uniqueId val="{00000000-44A2-4217-A4C2-1F7D4768DEA7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1169,16 +1140,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1339598912"/>
-        <c:axId val="1617722160"/>
+        <c:axId val="1419971056"/>
+        <c:axId val="1341957264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1339598912"/>
+        <c:axId val="1419971056"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="22000000"/>
-          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1196,67 +1164,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Frequency</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> (Hz)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -1293,12 +1201,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1617722160"/>
+        <c:crossAx val="1341957264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1617722160"/>
+        <c:axId val="1341957264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1318,61 +1226,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Amplitude (dB)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1410,7 +1263,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1339598912"/>
+        <c:crossAx val="1419971056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1481,31 +1334,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Filter phase response</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1537,17 +1365,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="8.9782696709298018E-2"/>
-          <c:y val="8.251558703860902E-2"/>
-          <c:w val="0.86020233979973437"/>
-          <c:h val="0.81042550907902311"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -1556,11 +1374,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Filter!$F$5</c:f>
+              <c:f>'ADC output response'!$I$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Phase</c:v>
+                  <c:v>RMS Peak dB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1579,7 +1397,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Filter!$C$6:$C$46</c:f>
+              <c:f>'ADC output response'!$H$6:$H$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1711,129 +1529,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Filter!$F$6:$F$46</c:f>
+              <c:f>'ADC output response'!$I$6:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>-47</c:v>
+                  <c:v>-6.9968813836281711</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40</c:v>
+                  <c:v>-6.2570577270670125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-34</c:v>
+                  <c:v>-5.7162558544986748</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-29</c:v>
+                  <c:v>-5.3169699337410172</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-24</c:v>
+                  <c:v>-5.0205569824330896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-20</c:v>
+                  <c:v>-4.8053138891567961</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-16</c:v>
+                  <c:v>-4.6563778720896023</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-13</c:v>
+                  <c:v>-4.5527882784722333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-10</c:v>
+                  <c:v>-4.4791022168507117</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-8</c:v>
+                  <c:v>-4.4328357047181743</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-7</c:v>
+                  <c:v>-4.4024160873730631</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-5</c:v>
+                  <c:v>-4.3819364333382698</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-4</c:v>
+                  <c:v>-4.3772337979238243</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2</c:v>
+                  <c:v>-4.3613470905680334</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-4.3571002378783232</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>-4.3552213812456584</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>-4.3545617264619256</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>-4.3568133632483965</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6</c:v>
+                  <c:v>-4.3614475480326194</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8</c:v>
+                  <c:v>-4.3692006278811659</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9</c:v>
+                  <c:v>-4.3809007720735806</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11</c:v>
+                  <c:v>-4.390715744218971</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>14</c:v>
+                  <c:v>-4.4256183808817449</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17</c:v>
+                  <c:v>-4.4648724980442598</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20</c:v>
+                  <c:v>-4.5257481196438594</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>24</c:v>
+                  <c:v>-4.6097358701668947</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>30</c:v>
+                  <c:v>-4.7262151911145676</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>35</c:v>
+                  <c:v>-4.8867249501167009</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43</c:v>
+                  <c:v>-5.098972844113062</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>49</c:v>
+                  <c:v>-5.3694172750400702</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>60</c:v>
+                  <c:v>-5.6763926785709415</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>68</c:v>
+                  <c:v>-6.0053435257347711</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>80</c:v>
+                  <c:v>-6.2839116848584142</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>95</c:v>
+                  <c:v>-6.3872715345177777</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>115</c:v>
+                  <c:v>-6.1589326993183846</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>146</c:v>
+                  <c:v>-5.6738050559034505</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-170</c:v>
+                  <c:v>-6.1066327110743348</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-117</c:v>
+                  <c:v>-7.8296932692592929</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>33</c:v>
+                  <c:v>-7.1857612109861133</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>60</c:v>
+                  <c:v>-34.240831882796982</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-58.547650469095267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1841,7 +1662,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0644-4DE4-9085-1C09BFAB8392}"/>
+              <c16:uniqueId val="{00000000-FFD8-49A0-902A-E403187A683F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1853,19 +1674,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1338956304"/>
-        <c:axId val="1617716112"/>
+        <c:axId val="1419966896"/>
+        <c:axId val="1341985776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1338956304"/>
+        <c:axId val="1419966896"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="22000000"/>
-          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="t"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1880,73 +1698,10 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Frequency (Hz)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.43859244595566882"/>
-              <c:y val="0.93519675282225412"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="high"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1980,16 +1735,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1617716112"/>
+        <c:crossAx val="1341985776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1617716112"/>
+        <c:axId val="1341985776"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
-          <c:max val="180"/>
-          <c:min val="-180"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2007,61 +1760,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Phase (degrees)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2099,7 +1797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1338956304"/>
+        <c:crossAx val="1419966896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3870,23 +3568,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>4761</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFCE856-F5C3-4DB1-A5D9-6BC5C6C547ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1CAC825-70B8-4B8D-A4E4-997F29B6D7E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3906,23 +3604,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB14326B-31B5-4489-8531-16DA35C85947}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DAAAB98-A52A-4F70-B367-0BFC9C691E80}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3941,26 +3639,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96140FBA-480D-4BF6-B0B9-5F38600184F9}" name="Table2" displayName="Table2" ref="B5:F46" totalsRowShown="0">
-  <autoFilter ref="B5:F46" xr:uid="{350EAA1F-12FF-4FCD-B71B-F94E77BA9594}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A70284C1-E80D-4A48-AFFC-1809B06CFC86}" name="Log10">
-      <calculatedColumnFormula>B5 + (1/12)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{DC4E205A-4452-4215-B462-9FA2CDDDD201}" name="Hz">
-      <calculatedColumnFormula xml:space="preserve"> ROUNDUP(10 ^ B6, 0)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{3C366408-4A01-4F38-87AA-2A3C31477FD3}" name="Amplitude"/>
-    <tableColumn id="4" xr3:uid="{9B7FDE06-47E8-4787-B4F9-EE412CAFE2F9}" name="Gain (dB)" dataDxfId="0">
-      <calculatedColumnFormula>20*LOG10(D6 / $D$2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{268775CA-9D02-490D-8233-D0A8E7F2DE25}" name="Phase"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4262,7 +3940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5473A75-8EE1-4908-A621-0E8DCAAAB26F}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
@@ -4274,12 +3952,12 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -4306,24 +3984,24 @@
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="P4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="R4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>1500</v>
@@ -5212,901 +4890,1162 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696FC061-23D0-40B8-BFCA-2B0991513C23}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="B2:K46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD30CAC2-A55D-4F1C-AF59-F3E4F91421B5}">
+  <dimension ref="B2:J46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA28" sqref="AA28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" customWidth="1"/>
-    <col min="22" max="22" width="12" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2010</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="D6" s="7">
         <f xml:space="preserve"> ROUNDUP(10 ^ B6, 0)</f>
         <v>10000</v>
       </c>
-      <c r="D6">
-        <v>1530</v>
-      </c>
       <c r="E6">
-        <f t="shared" ref="E6:E46" si="0">20*LOG10(D6 / $D$2)</f>
-        <v>-2.3700925320578019</v>
-      </c>
-      <c r="F6">
-        <v>-47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F6 / 1)</f>
+        <v>-3.9569408226557687</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.63409300000000002</v>
+      </c>
+      <c r="H6">
+        <v>10000</v>
+      </c>
+      <c r="I6">
+        <f>20*LOG10(J6 / 1)</f>
+        <v>-6.9968813836281711</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.44684400000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f t="shared" ref="B6:B12" si="1">B6 + (1/12)</f>
+        <f t="shared" ref="B7:B12" si="0">B6 + (1/12)</f>
         <v>4.083333333333333</v>
       </c>
-      <c r="C7">
-        <f t="shared" ref="C7:C60" si="2" xml:space="preserve"> ROUNDUP(10 ^ B7, 0)</f>
+      <c r="D7" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B7, 0)</f>
         <v>12116</v>
       </c>
-      <c r="D7" s="1">
-        <v>1650</v>
-      </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>-1.7142422641316513</v>
-      </c>
-      <c r="F7">
-        <v>-40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F7 / 1)</f>
+        <v>-3.216889871943414</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.69048699999999996</v>
+      </c>
+      <c r="H7">
+        <v>12116</v>
+      </c>
+      <c r="I7">
+        <f>20*LOG10(J7 / 1)</f>
+        <v>-6.2570577270670125</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.486572</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.1666666666666661</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="2"/>
+      <c r="D8" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B8, 0)</f>
         <v>14678</v>
       </c>
-      <c r="D8" s="1">
-        <v>1750</v>
-      </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>-1.2031601746838883</v>
-      </c>
-      <c r="F8">
-        <v>-34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F8 / 1)</f>
+        <v>-2.6692558380816345</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.73542300000000005</v>
+      </c>
+      <c r="H8">
+        <v>14678</v>
+      </c>
+      <c r="I8">
+        <f>20*LOG10(J8 / 1)</f>
+        <v>-5.7162558544986748</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.51783000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.2499999999999991</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="2"/>
+      <c r="D9" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B9, 0)</f>
         <v>17783</v>
       </c>
-      <c r="D9" s="1">
-        <v>1810</v>
-      </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>-0.91034965102608711</v>
-      </c>
-      <c r="F9">
-        <v>-29</v>
-      </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F9 / 1)</f>
+        <v>-2.2637580608355079</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.77056999999999998</v>
+      </c>
+      <c r="H9">
+        <v>17783</v>
+      </c>
+      <c r="I9">
+        <f>20*LOG10(J9 / 1)</f>
+        <v>-5.3169699337410172</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.54218999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.3333333333333321</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="2"/>
+      <c r="D10" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B10, 0)</f>
         <v>21545</v>
       </c>
-      <c r="D10" s="1">
-        <v>1870</v>
-      </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>-0.62708901767979819</v>
-      </c>
-      <c r="F10">
-        <v>-24</v>
-      </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F10 / 1)</f>
+        <v>-1.9809312005754807</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.79607399999999995</v>
+      </c>
+      <c r="H10">
+        <v>21545</v>
+      </c>
+      <c r="I10">
+        <f>20*LOG10(J10 / 1)</f>
+        <v>-5.0205569824330896</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.56101199999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.4166666666666652</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="2"/>
+      <c r="D11" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B11, 0)</f>
         <v>26102</v>
       </c>
-      <c r="D11" s="1">
-        <v>1910</v>
-      </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>-0.44325380345522664</v>
-      </c>
-      <c r="F11">
-        <v>-20</v>
-      </c>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F11 / 1)</f>
+        <v>-1.7481837792480062</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.81769400000000003</v>
+      </c>
+      <c r="H11">
+        <v>26102</v>
+      </c>
+      <c r="I11">
+        <f>20*LOG10(J11 / 1)</f>
+        <v>-4.8053138891567961</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.57508800000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.4999999999999982</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="2"/>
+      <c r="D12" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B12, 0)</f>
         <v>31623</v>
       </c>
-      <c r="D12" s="1">
-        <v>1950</v>
-      </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>-0.26322892115941698</v>
-      </c>
-      <c r="F12">
-        <v>-16</v>
-      </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F12 / 1)</f>
+        <v>-1.6038936228528302</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.83139099999999999</v>
+      </c>
+      <c r="H12">
+        <v>31623</v>
+      </c>
+      <c r="I12">
+        <f>20*LOG10(J12 / 1)</f>
+        <v>-4.6563778720896023</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.58503400000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>B12 + (1/12)</f>
         <v>4.5833333333333313</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="2"/>
+      <c r="D13" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B13, 0)</f>
         <v>38312</v>
       </c>
-      <c r="D13" s="1">
-        <v>1970</v>
-      </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>-0.17459662517791907</v>
-      </c>
-      <c r="F13">
-        <v>-13</v>
-      </c>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F13 / 1)</f>
+        <v>-1.5024380793839742</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.84115899999999999</v>
+      </c>
+      <c r="H13">
+        <v>38312</v>
+      </c>
+      <c r="I13">
+        <f>20*LOG10(J13 / 1)</f>
+        <v>-4.5527882784722333</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.59205300000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f t="shared" ref="B14:B26" si="3">B13 + (1/12)</f>
+        <f t="shared" ref="B14:B26" si="1">B13 + (1/12)</f>
         <v>4.6666666666666643</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="2"/>
+      <c r="D14" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B14, 0)</f>
         <v>46416</v>
       </c>
-      <c r="D14" s="1">
-        <v>1990</v>
-      </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>-8.6859620215644029E-2</v>
-      </c>
-      <c r="F14">
-        <v>-10</v>
-      </c>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F14 / 1)</f>
+        <v>-1.4222452027494425</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.84896099999999997</v>
+      </c>
+      <c r="H14">
+        <v>46416</v>
+      </c>
+      <c r="I14">
+        <f>20*LOG10(J14 / 1)</f>
+        <v>-4.4791022168507117</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.59709699999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4.7499999999999973</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="2"/>
+      <c r="D15" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B15, 0)</f>
         <v>56235</v>
       </c>
-      <c r="D15" s="1">
-        <v>1990</v>
-      </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>-8.6859620215644029E-2</v>
-      </c>
-      <c r="F15">
-        <v>-8</v>
-      </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F15 / 1)</f>
+        <v>-1.3891388258243724</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.85220300000000004</v>
+      </c>
+      <c r="H15">
+        <v>56235</v>
+      </c>
+      <c r="I15">
+        <f>20*LOG10(J15 / 1)</f>
+        <v>-4.4328357047181743</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.60028599999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4.8333333333333304</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="2"/>
+      <c r="D16" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B16, 0)</f>
         <v>68130</v>
       </c>
-      <c r="D16" s="1">
-        <v>2010</v>
-      </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>-7</v>
-      </c>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F16 / 1)</f>
+        <v>-1.3487998762784796</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.85616999999999999</v>
+      </c>
+      <c r="H16">
+        <v>68130</v>
+      </c>
+      <c r="I16">
+        <f>20*LOG10(J16 / 1)</f>
+        <v>-4.4024160873730631</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.60239200000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4.9166666666666634</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="2"/>
+      <c r="D17" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B17, 0)</f>
         <v>82541</v>
       </c>
-      <c r="D17" s="1">
-        <v>2010</v>
-      </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>-5</v>
-      </c>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F17 / 1)</f>
+        <v>-1.3290293962371769</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.85812100000000002</v>
+      </c>
+      <c r="H17">
+        <v>82541</v>
+      </c>
+      <c r="I17">
+        <f>20*LOG10(J17 / 1)</f>
+        <v>-4.3819364333382698</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.60381399999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4.9999999999999964</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="2"/>
+      <c r="D18" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B18, 0)</f>
         <v>100000</v>
       </c>
-      <c r="D18" s="1">
-        <v>2010</v>
-      </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>-4</v>
-      </c>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F18 / 1)</f>
+        <v>-1.3231403965924835</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.85870299999999999</v>
+      </c>
+      <c r="H18">
+        <v>100000</v>
+      </c>
+      <c r="I18">
+        <f>20*LOG10(J18 / 1)</f>
+        <v>-4.3772337979238243</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.60414100000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.0833333333333295</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="2"/>
+      <c r="D19" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B19, 0)</f>
         <v>121153</v>
       </c>
-      <c r="D19" s="1">
-        <v>2010</v>
-      </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>-2</v>
-      </c>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F19 / 1)</f>
+        <v>-1.3096976857579279</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.86003300000000005</v>
+      </c>
+      <c r="H19">
+        <v>121153</v>
+      </c>
+      <c r="I19">
+        <f>20*LOG10(J19 / 1)</f>
+        <v>-4.3613470905680334</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0.60524699999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.1666666666666625</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="2"/>
+      <c r="D20" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B20, 0)</f>
         <v>146780</v>
       </c>
-      <c r="D20" s="1">
-        <v>2010</v>
-      </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F20 / 1)</f>
+        <v>-1.3093543100847316</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.86006700000000003</v>
+      </c>
+      <c r="H20">
+        <v>146780</v>
+      </c>
+      <c r="I20">
+        <f>20*LOG10(J20 / 1)</f>
+        <v>-4.3571002378783232</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.60554300000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.2499999999999956</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
+      <c r="D21" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B21, 0)</f>
         <v>177828</v>
       </c>
-      <c r="D21" s="1">
-        <v>2010</v>
-      </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F21 / 1)</f>
+        <v>-1.3036703854417109</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.86063000000000001</v>
+      </c>
+      <c r="H21">
+        <v>177828</v>
+      </c>
+      <c r="I21">
+        <f>20*LOG10(J21 / 1)</f>
+        <v>-4.3552213812456584</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0.60567400000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.3333333333333286</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="2"/>
+      <c r="D22" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B22, 0)</f>
         <v>215444</v>
       </c>
-      <c r="D22" s="1">
-        <v>2010</v>
-      </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F22 / 1)</f>
+        <v>-1.3035290918940998</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.86064399999999996</v>
+      </c>
+      <c r="H22">
+        <v>215444</v>
+      </c>
+      <c r="I22">
+        <f>20*LOG10(J22 / 1)</f>
+        <v>-4.3545617264619256</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0.60572000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.4166666666666616</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="2"/>
+      <c r="D23" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B23, 0)</f>
         <v>261016</v>
       </c>
-      <c r="D23" s="1">
-        <v>2010</v>
-      </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>4</v>
-      </c>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F23 / 1)</f>
+        <v>-1.3037208479800224</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.86062499999999997</v>
+      </c>
+      <c r="H23">
+        <v>261016</v>
+      </c>
+      <c r="I23">
+        <f>20*LOG10(J23 / 1)</f>
+        <v>-4.3568133632483965</v>
+      </c>
+      <c r="J23" s="8">
+        <v>0.60556299999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.4999999999999947</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="2"/>
+      <c r="D24" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B24, 0)</f>
         <v>316228</v>
       </c>
-      <c r="D24" s="1">
-        <v>2010</v>
-      </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>6</v>
-      </c>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F24 / 1)</f>
+        <v>-1.3090210466770615</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.86009999999999998</v>
+      </c>
+      <c r="H24">
+        <v>316228</v>
+      </c>
+      <c r="I24">
+        <f>20*LOG10(J24 / 1)</f>
+        <v>-4.3614475480326194</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0.60524</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.5833333333333277</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="2"/>
+      <c r="D25" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B25, 0)</f>
         <v>383119</v>
       </c>
-      <c r="D25" s="1">
-        <v>2010</v>
-      </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>8</v>
-      </c>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F25 / 1)</f>
+        <v>-1.3238484843225506</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.85863299999999998</v>
+      </c>
+      <c r="H25">
+        <v>383119</v>
+      </c>
+      <c r="I25">
+        <f>20*LOG10(J25 / 1)</f>
+        <v>-4.3692006278811659</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0.60470000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5.6666666666666607</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="2"/>
+      <c r="D26" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B26, 0)</f>
         <v>464159</v>
       </c>
-      <c r="D26" s="1">
-        <v>2010</v>
-      </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>9</v>
-      </c>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+        <f>20*LOG10(F26 / 1)</f>
+        <v>-1.3288573241619814</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.85813799999999996</v>
+      </c>
+      <c r="H26">
+        <v>464159</v>
+      </c>
+      <c r="I26">
+        <f>20*LOG10(J26 / 1)</f>
+        <v>-4.3809007720735806</v>
+      </c>
+      <c r="J26" s="8">
+        <v>0.60388600000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>B26 + (1/12)</f>
         <v>5.7499999999999938</v>
       </c>
-      <c r="C27">
+      <c r="D27" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B27, 0)</f>
+        <v>562342</v>
+      </c>
+      <c r="E27">
+        <f>20*LOG10(F27 / 1)</f>
+        <v>-1.3437288305971651</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.85667000000000004</v>
+      </c>
+      <c r="H27">
+        <v>562342</v>
+      </c>
+      <c r="I27">
+        <f>20*LOG10(J27 / 1)</f>
+        <v>-4.390715744218971</v>
+      </c>
+      <c r="J27" s="8">
+        <v>0.60320399999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" ref="B28:B46" si="2">B27 + (1/12)</f>
+        <v>5.8333333333333268</v>
+      </c>
+      <c r="D28" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B28, 0)</f>
+        <v>681293</v>
+      </c>
+      <c r="E28">
+        <f>20*LOG10(F28 / 1)</f>
+        <v>-1.3680765606671534</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.85427200000000003</v>
+      </c>
+      <c r="H28">
+        <v>681293</v>
+      </c>
+      <c r="I28">
+        <f>20*LOG10(J28 / 1)</f>
+        <v>-4.4256183808817449</v>
+      </c>
+      <c r="J28" s="8">
+        <v>0.60078500000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29">
         <f t="shared" si="2"/>
-        <v>562342</v>
-      </c>
-      <c r="D27">
-        <v>2010</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>11</v>
-      </c>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <f t="shared" ref="B28:B46" si="4">B27 + (1/12)</f>
-        <v>5.8333333333333268</v>
-      </c>
-      <c r="C28">
+        <v>5.9166666666666599</v>
+      </c>
+      <c r="D29" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B29, 0)</f>
+        <v>825405</v>
+      </c>
+      <c r="E29">
+        <f>20*LOG10(F29 / 1)</f>
+        <v>-1.4233093127111565</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.84885699999999997</v>
+      </c>
+      <c r="H29">
+        <v>825405</v>
+      </c>
+      <c r="I29">
+        <f>20*LOG10(J29 / 1)</f>
+        <v>-4.4648724980442598</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0.59807600000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30">
         <f t="shared" si="2"/>
-        <v>681293</v>
-      </c>
-      <c r="D28">
-        <v>1990</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>-8.6859620215644029E-2</v>
-      </c>
-      <c r="F28">
-        <v>14</v>
-      </c>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <f t="shared" si="4"/>
-        <v>5.9166666666666599</v>
-      </c>
-      <c r="C29">
+        <v>5.9999999999999929</v>
+      </c>
+      <c r="D30" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B30, 0)</f>
+        <v>1000000</v>
+      </c>
+      <c r="E30">
+        <f>20*LOG10(F30 / 1)</f>
+        <v>-1.4675646675716463</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.84454300000000004</v>
+      </c>
+      <c r="H30">
+        <v>1000000</v>
+      </c>
+      <c r="I30">
+        <f>20*LOG10(J30 / 1)</f>
+        <v>-4.5257481196438594</v>
+      </c>
+      <c r="J30" s="8">
+        <v>0.59389899999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31">
         <f t="shared" si="2"/>
-        <v>825405</v>
-      </c>
-      <c r="D29">
-        <v>1990</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>-8.6859620215644029E-2</v>
-      </c>
-      <c r="F29">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <f t="shared" si="4"/>
-        <v>5.9999999999999929</v>
-      </c>
-      <c r="C30">
+        <v>6.0833333333333259</v>
+      </c>
+      <c r="D31" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B31, 0)</f>
+        <v>1211528</v>
+      </c>
+      <c r="E31">
+        <f>20*LOG10(F31 / 1)</f>
+        <v>-1.5653551394136862</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.83508800000000005</v>
+      </c>
+      <c r="H31">
+        <v>1211528</v>
+      </c>
+      <c r="I31">
+        <f>20*LOG10(J31 / 1)</f>
+        <v>-4.6097358701668947</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0.58818400000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32">
         <f t="shared" si="2"/>
-        <v>1000000</v>
-      </c>
-      <c r="D30">
-        <v>1970</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>-0.17459662517791907</v>
-      </c>
-      <c r="F30">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <f t="shared" si="4"/>
-        <v>6.0833333333333259</v>
-      </c>
-      <c r="C31">
+        <v>6.166666666666659</v>
+      </c>
+      <c r="D32" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B32, 0)</f>
+        <v>1467800</v>
+      </c>
+      <c r="E32">
+        <f>20*LOG10(F32 / 1)</f>
+        <v>-1.6677841468865393</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.82529799999999998</v>
+      </c>
+      <c r="H32">
+        <v>1467800</v>
+      </c>
+      <c r="I32">
+        <f>20*LOG10(J32 / 1)</f>
+        <v>-4.7262151911145676</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0.580349</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33">
         <f t="shared" si="2"/>
-        <v>1211528</v>
-      </c>
-      <c r="D31">
-        <v>1950</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>-0.26322892115941698</v>
-      </c>
-      <c r="F31">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <f t="shared" si="4"/>
-        <v>6.166666666666659</v>
-      </c>
-      <c r="C32">
+        <v>6.249999999999992</v>
+      </c>
+      <c r="D33" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B33, 0)</f>
+        <v>1778280</v>
+      </c>
+      <c r="E33">
+        <f>20*LOG10(F33 / 1)</f>
+        <v>-1.8342359728863094</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0.80963300000000005</v>
+      </c>
+      <c r="H33">
+        <v>1778280</v>
+      </c>
+      <c r="I33">
+        <f>20*LOG10(J33 / 1)</f>
+        <v>-4.8867249501167009</v>
+      </c>
+      <c r="J33" s="8">
+        <v>0.56972299999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34">
         <f t="shared" si="2"/>
-        <v>1467800</v>
-      </c>
-      <c r="D32">
-        <v>1930</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>-0.35277496825430255</v>
-      </c>
-      <c r="F32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <f t="shared" si="4"/>
-        <v>6.249999999999992</v>
-      </c>
-      <c r="C33">
+        <v>6.333333333333325</v>
+      </c>
+      <c r="D34" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B34, 0)</f>
+        <v>2154435</v>
+      </c>
+      <c r="E34">
+        <f>20*LOG10(F34 / 1)</f>
+        <v>-2.0469414341029211</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.79004700000000005</v>
+      </c>
+      <c r="H34">
+        <v>2154435</v>
+      </c>
+      <c r="I34">
+        <f>20*LOG10(J34 / 1)</f>
+        <v>-5.098972844113062</v>
+      </c>
+      <c r="J34" s="8">
+        <v>0.55596999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35">
         <f t="shared" si="2"/>
-        <v>1778280</v>
-      </c>
-      <c r="D33">
-        <v>1910</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>-0.44325380345522664</v>
-      </c>
-      <c r="F33">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <f t="shared" si="4"/>
-        <v>6.333333333333325</v>
-      </c>
-      <c r="C34">
+        <v>6.4166666666666581</v>
+      </c>
+      <c r="D35" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B35, 0)</f>
+        <v>2610158</v>
+      </c>
+      <c r="E35">
+        <f>20*LOG10(F35 / 1)</f>
+        <v>-2.3293377035635094</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0.76477399999999995</v>
+      </c>
+      <c r="H35">
+        <v>2610158</v>
+      </c>
+      <c r="I35">
+        <f>20*LOG10(J35 / 1)</f>
+        <v>-5.3694172750400702</v>
+      </c>
+      <c r="J35" s="8">
+        <v>0.53892600000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36">
         <f t="shared" si="2"/>
-        <v>2154435</v>
-      </c>
-      <c r="D34">
-        <v>1870</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>-0.62708901767979819</v>
-      </c>
-      <c r="F34">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <f t="shared" si="4"/>
-        <v>6.4166666666666581</v>
-      </c>
-      <c r="C35">
+        <v>6.4999999999999911</v>
+      </c>
+      <c r="D36" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B36, 0)</f>
+        <v>3162278</v>
+      </c>
+      <c r="E36">
+        <f>20*LOG10(F36 / 1)</f>
+        <v>-2.6237151138378687</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.73928899999999997</v>
+      </c>
+      <c r="H36">
+        <v>3162278</v>
+      </c>
+      <c r="I36">
+        <f>20*LOG10(J36 / 1)</f>
+        <v>-5.6763926785709415</v>
+      </c>
+      <c r="J36" s="8">
+        <v>0.52021200000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37">
         <f t="shared" si="2"/>
-        <v>2610158</v>
-      </c>
-      <c r="D35">
-        <v>1810</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>-0.91034965102608711</v>
-      </c>
-      <c r="F35">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <f t="shared" si="4"/>
-        <v>6.4999999999999911</v>
-      </c>
-      <c r="C36">
+        <v>6.5833333333333242</v>
+      </c>
+      <c r="D37" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B37, 0)</f>
+        <v>3831187</v>
+      </c>
+      <c r="E37">
+        <f>20*LOG10(F37 / 1)</f>
+        <v>-2.9746617562437736</v>
+      </c>
+      <c r="F37" s="8">
+        <v>0.71001400000000003</v>
+      </c>
+      <c r="H37">
+        <v>3831187</v>
+      </c>
+      <c r="I37">
+        <f>20*LOG10(J37 / 1)</f>
+        <v>-6.0053435257347711</v>
+      </c>
+      <c r="J37" s="8">
+        <v>0.50087899999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38">
         <f t="shared" si="2"/>
-        <v>3162278</v>
-      </c>
-      <c r="D36">
-        <v>1750</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>-1.2031601746838883</v>
-      </c>
-      <c r="F36">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <f t="shared" si="4"/>
-        <v>6.5833333333333242</v>
-      </c>
-      <c r="C37">
+        <v>6.6666666666666572</v>
+      </c>
+      <c r="D38" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B38, 0)</f>
+        <v>4641589</v>
+      </c>
+      <c r="E38">
+        <f>20*LOG10(F38 / 1)</f>
+        <v>-3.2668855156566847</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0.68652400000000002</v>
+      </c>
+      <c r="H38">
+        <v>4641589</v>
+      </c>
+      <c r="I38">
+        <f>20*LOG10(J38 / 1)</f>
+        <v>-6.2839116848584142</v>
+      </c>
+      <c r="J38" s="8">
+        <v>0.48507</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39">
         <f t="shared" si="2"/>
-        <v>3831187</v>
-      </c>
-      <c r="D37">
-        <v>1710</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>-1.4039989405667006</v>
-      </c>
-      <c r="F37">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <f t="shared" si="4"/>
-        <v>6.6666666666666572</v>
-      </c>
-      <c r="C38">
+        <v>6.7499999999999902</v>
+      </c>
+      <c r="D39" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B39, 0)</f>
+        <v>5623414</v>
+      </c>
+      <c r="E39">
+        <f>20*LOG10(F39 / 1)</f>
+        <v>-3.3406935865431637</v>
+      </c>
+      <c r="F39" s="8">
+        <v>0.68071499999999996</v>
+      </c>
+      <c r="H39">
+        <v>5623414</v>
+      </c>
+      <c r="I39">
+        <f>20*LOG10(J39 / 1)</f>
+        <v>-6.3872715345177777</v>
+      </c>
+      <c r="J39" s="8">
+        <v>0.47933199999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40">
         <f t="shared" si="2"/>
-        <v>4641589</v>
-      </c>
-      <c r="D38">
-        <v>1650</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
-        <v>-1.7142422641316513</v>
-      </c>
-      <c r="F38">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <f t="shared" si="4"/>
-        <v>6.7499999999999902</v>
-      </c>
-      <c r="C39">
+        <v>6.8333333333333233</v>
+      </c>
+      <c r="D40" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B40, 0)</f>
+        <v>6812921</v>
+      </c>
+      <c r="E40">
+        <f>20*LOG10(F40 / 1)</f>
+        <v>-3.0944291016408734</v>
+      </c>
+      <c r="F40" s="8">
+        <v>0.700291</v>
+      </c>
+      <c r="H40">
+        <v>6812921</v>
+      </c>
+      <c r="I40">
+        <f>20*LOG10(J40 / 1)</f>
+        <v>-6.1589326993183846</v>
+      </c>
+      <c r="J40" s="8">
+        <v>0.49209999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41">
         <f t="shared" si="2"/>
-        <v>5623414</v>
-      </c>
-      <c r="D39">
-        <v>1650</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>-1.7142422641316513</v>
-      </c>
-      <c r="F39">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <f t="shared" si="4"/>
-        <v>6.8333333333333233</v>
-      </c>
-      <c r="C40">
+        <v>6.9166666666666563</v>
+      </c>
+      <c r="D41" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B41, 0)</f>
+        <v>8254042</v>
+      </c>
+      <c r="E41">
+        <f>20*LOG10(F41 / 1)</f>
+        <v>-2.6229632118397062</v>
+      </c>
+      <c r="F41" s="8">
+        <v>0.73935300000000004</v>
+      </c>
+      <c r="H41">
+        <v>8254042</v>
+      </c>
+      <c r="I41">
+        <f>20*LOG10(J41 / 1)</f>
+        <v>-5.6738050559034505</v>
+      </c>
+      <c r="J41" s="8">
+        <v>0.52036700000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42">
         <f t="shared" si="2"/>
-        <v>6812921</v>
-      </c>
-      <c r="D40">
-        <v>1730</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>-1.3029990858338694</v>
-      </c>
-      <c r="F40">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <f t="shared" si="4"/>
-        <v>6.9166666666666563</v>
-      </c>
-      <c r="C41">
+        <v>6.9999999999999893</v>
+      </c>
+      <c r="D42" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B42, 0)</f>
+        <v>10000000</v>
+      </c>
+      <c r="E42">
+        <f>20*LOG10(F42 / 1)</f>
+        <v>-3.0480039660192979</v>
+      </c>
+      <c r="F42" s="8">
+        <v>0.704044</v>
+      </c>
+      <c r="H42">
+        <v>10000000</v>
+      </c>
+      <c r="I42">
+        <f>20*LOG10(J42 / 1)</f>
+        <v>-6.1066327110743348</v>
+      </c>
+      <c r="J42" s="8">
+        <v>0.49507200000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43">
         <f t="shared" si="2"/>
-        <v>8254042</v>
-      </c>
-      <c r="D41">
-        <v>1890</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
-        <v>-0.5346850649448941</v>
-      </c>
-      <c r="F41">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <f t="shared" si="4"/>
-        <v>6.9999999999999893</v>
-      </c>
-      <c r="C42">
+        <v>7.0833333333333224</v>
+      </c>
+      <c r="D43" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B43, 0)</f>
+        <v>12115277</v>
+      </c>
+      <c r="E43">
+        <f>20*LOG10(F43 / 1)</f>
+        <v>-4.7399954493073375</v>
+      </c>
+      <c r="F43" s="8">
+        <v>0.57942899999999997</v>
+      </c>
+      <c r="H43">
+        <v>12115277</v>
+      </c>
+      <c r="I43">
+        <f>20*LOG10(J43 / 1)</f>
+        <v>-7.8296932692592929</v>
+      </c>
+      <c r="J43" s="8">
+        <v>0.40599000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44">
         <f t="shared" si="2"/>
-        <v>10000000</v>
-      </c>
-      <c r="D42">
-        <v>1850</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
-        <v>-0.72048658034950108</v>
-      </c>
-      <c r="F42">
-        <v>-170</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <f t="shared" si="4"/>
-        <v>7.0833333333333224</v>
-      </c>
-      <c r="C43">
+        <v>7.1666666666666554</v>
+      </c>
+      <c r="D44" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B44, 0)</f>
+        <v>14677993</v>
+      </c>
+      <c r="E44">
+        <f>20*LOG10(F44 / 1)</f>
+        <v>-4.0375159626601489</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.62823799999999996</v>
+      </c>
+      <c r="H44">
+        <v>14677993</v>
+      </c>
+      <c r="I44">
+        <f>20*LOG10(J44 / 1)</f>
+        <v>-7.1857612109861133</v>
+      </c>
+      <c r="J44" s="8">
+        <v>0.43723200000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45">
         <f t="shared" si="2"/>
-        <v>12115277</v>
-      </c>
-      <c r="D43">
-        <v>1690</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
-        <v>-1.5061870561363073</v>
-      </c>
-      <c r="F43">
-        <v>-117</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <f t="shared" si="4"/>
-        <v>7.1666666666666554</v>
-      </c>
-      <c r="C44">
+        <v>7.2499999999999885</v>
+      </c>
+      <c r="D45" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B45, 0)</f>
+        <v>17782795</v>
+      </c>
+      <c r="E45">
+        <f>20*LOG10(F45 / 1)</f>
+        <v>-29.729522077725093</v>
+      </c>
+      <c r="F45" s="8">
+        <v>3.2622999999999999E-2</v>
+      </c>
+      <c r="H45">
+        <v>17782795</v>
+      </c>
+      <c r="I45">
+        <f>20*LOG10(J45 / 1)</f>
+        <v>-34.240831882796982</v>
+      </c>
+      <c r="J45" s="8">
+        <v>1.9407000000000001E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46">
         <f t="shared" si="2"/>
-        <v>14677993</v>
-      </c>
-      <c r="D44">
-        <v>820</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
-        <v>-7.7876441007354451</v>
-      </c>
-      <c r="F44">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <f t="shared" si="4"/>
-        <v>7.2499999999999885</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="2"/>
-        <v>17782795</v>
-      </c>
-      <c r="D45">
-        <v>48</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
-        <v>-32.43909640089803</v>
-      </c>
-      <c r="F45">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <f t="shared" si="4"/>
         <v>7.3333333333333215</v>
       </c>
-      <c r="C46">
-        <f t="shared" si="2"/>
+      <c r="D46" s="7">
+        <f xml:space="preserve"> ROUNDUP(10 ^ B46, 0)</f>
         <v>21544347</v>
       </c>
-      <c r="D46">
-        <v>32</v>
-      </c>
       <c r="E46">
-        <f t="shared" si="0"/>
-        <v>-35.960921582011657</v>
+        <f>20*LOG10(F46 / 1)</f>
+        <v>-43.521390897488729</v>
+      </c>
+      <c r="F46" s="8">
+        <v>6.6670000000000002E-3</v>
+      </c>
+      <c r="H46">
+        <v>21544347</v>
+      </c>
+      <c r="I46">
+        <f>20*LOG10(J46 / 1)</f>
+        <v>-58.547650469095267</v>
+      </c>
+      <c r="J46" s="8">
+        <v>1.1820000000000001E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved filter phase-shift analysis
</commit_message>
<xml_diff>
--- a/Documentation/DdD Gain and filter calculations.xlsx
+++ b/Documentation/DdD Gain and filter calculations.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simon\Documents\GitHub\DomesdayDuplicator\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57C222A-20AF-46A3-BC3A-480552E17691}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7089AA06-0089-4023-897F-9DBED4C9683F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="38400" windowHeight="17610" activeTab="1" xr2:uid="{6586ADF8-B05F-4BD6-A150-BEC042DE64BB}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="38400" windowHeight="17610" activeTab="1" xr2:uid="{6586ADF8-B05F-4BD6-A150-BEC042DE64BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequency Response" sheetId="3" r:id="rId1"/>
-    <sheet name="Phase shift" sheetId="4" r:id="rId2"/>
+    <sheet name="Phase shift" sheetId="5" r:id="rId2"/>
     <sheet name="Gain Setting" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Hz</t>
   </si>
@@ -77,13 +77,7 @@
     <t>Note: 0dB is relative to ADC maximum</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Phase (deg)</t>
-  </si>
-  <si>
-    <t>Measured from BNC input to ADC input @ 200mVPP 50 Ohms</t>
+    <t>Phase</t>
   </si>
 </sst>
 </file>
@@ -1286,6 +1280,1421 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Phase (Linear)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Phase shift'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Phase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Phase shift'!$B$5:$B$69</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1750000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2250000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2750000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3250000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3500000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3750000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4250000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4500000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4750000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5250000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5500000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5750000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6250000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6500000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6750000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7250000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7750000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8250000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8500000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8750000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9250000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9500000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9750000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10250000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10500000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10750000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11000000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11250000</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11500000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11750000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12000000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12250000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12500000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12750000</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>13000000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>13250000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>13500000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>13750000</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>14000000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>14250000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14500000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>14750000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>15000000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>15250000</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>15500000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>15750000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Phase shift'!$C$5:$C$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6960000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38.96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46.43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.31</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55.13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59.42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67.430000000000007</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>73.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>73.81</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>81.44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>89.44</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>95.54</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>99.01</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>109.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>113.7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>114.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>121.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>125.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>130.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>146.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>153.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>162.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>165.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>172.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>176.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>188.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>199.7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>205.6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>214.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>218.7</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>226.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>233.7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>237.7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>249.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>254.2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>261.8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>263.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>269.3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>281.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>357.3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>36.6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>48.96</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>60.41</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>69.930000000000007</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>81.569999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D6DA-4B36-AE0B-1389224CA250}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="993010496"/>
+        <c:axId val="998625008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="993010496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="998625008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="998625008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="360"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="993010496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="45"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Phase (Log10)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Phase shift'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Phase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Phase shift'!$B$5:$B$69</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1750000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2250000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2500000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2750000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3250000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3500000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3750000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4250000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4500000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4750000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5250000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5500000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5750000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6250000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6500000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6750000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7250000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7750000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8000000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8250000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8500000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8750000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9000000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9250000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9500000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9750000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10250000</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10500000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10750000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11000000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11250000</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11500000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11750000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12000000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12250000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12500000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12750000</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>13000000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>13250000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>13500000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>13750000</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>14000000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>14250000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14500000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>14750000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>15000000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>15250000</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>15500000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>15750000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>16000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Phase shift'!$C$5:$C$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6960000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38.96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46.43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.31</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55.13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59.42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67.430000000000007</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>73.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>73.81</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>81.44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>89.44</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>95.54</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>99.01</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>109.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>113.7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>114.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>121.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>125.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>130.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>146.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>153.6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>162.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>165.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>172.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>176.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>188.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>199.7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>205.6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>214.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>218.7</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>226.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>233.7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>237.7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>249.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>254.2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>261.8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>263.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>269.3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>281.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>357.3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>36.6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>48.96</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>60.41</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>69.930000000000007</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>72.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>81.569999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B7C9-44BA-9DDA-2E81515E0964}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="900638928"/>
+        <c:axId val="884927648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="900638928"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="16000000"/>
+          <c:min val="100000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="884927648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="884927648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="360"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900638928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="45"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1987,6 +3396,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3020,6 +4509,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3616,6 +6137,83 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A330FE4-2D29-4173-A1DA-214D4A88D396}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD0AEBD5-48BC-4E9C-AA03-B1EBE8DC5585}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4762</xdr:colOff>
       <xdr:row>22</xdr:row>
@@ -3656,18 +6254,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{935ECE5F-E8D3-4733-A57B-05EBFA85FE57}" name="Table3" displayName="Table3" ref="B5:D46" totalsRowShown="0">
-  <autoFilter ref="B5:D46" xr:uid="{CB7EC39D-23DC-4B9E-95E1-AC73593DB634}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{43A68A91-268C-4CA1-89CE-EB0F1354C108}" name="Log10">
-      <calculatedColumnFormula>B5 + (1/12)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0202C8F1-EA86-414D-9CBE-6AC49980A1A0}" name="Table1" displayName="Table1" ref="B4:C69" totalsRowShown="0">
+  <autoFilter ref="B4:C69" xr:uid="{8EDF63C4-2FED-4553-91E3-15DB0C2D0663}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4EF13AD5-6517-4F1E-8CFF-01D0B78FDE86}" name="Hz" dataDxfId="0">
+      <calculatedColumnFormula>B4+250000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{67DB8C2C-8CA1-4673-83CE-7282A4396EC5}" name="Hz" dataDxfId="0">
-      <calculatedColumnFormula xml:space="preserve"> ROUNDUP(10 ^ B6, 0)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{82408428-9CBD-46D6-8289-DB17815ACCDE}" name="Phase (deg)"/>
+    <tableColumn id="2" xr3:uid="{C8C83ABE-680A-4539-BB32-4DE1FCFAC900}" name="Phase"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -5128,571 +7723,613 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F0855-7EC8-4C8D-A70E-3292D4976783}">
-  <dimension ref="B2:D46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A394E6D-CEB8-4484-94B7-171087126E49}">
+  <dimension ref="B4:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B6, 0)</f>
-        <v>10000</v>
-      </c>
-      <c r="D6">
-        <v>-50.199999999999989</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <f t="shared" ref="B7:B12" si="0">B6 + (1/12)</f>
-        <v>4.083333333333333</v>
-      </c>
-      <c r="C7" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B7, 0)</f>
-        <v>12116</v>
-      </c>
-      <c r="D7">
-        <v>-44.699999999999989</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666661</v>
-      </c>
-      <c r="C8" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B8, 0)</f>
-        <v>14678</v>
-      </c>
-      <c r="D8">
-        <v>-37.600000000000023</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>4.2499999999999991</v>
-      </c>
-      <c r="C9" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B9, 0)</f>
-        <v>17783</v>
-      </c>
-      <c r="D9">
-        <v>-30.5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>4.3333333333333321</v>
-      </c>
-      <c r="C10" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B10, 0)</f>
-        <v>21545</v>
-      </c>
-      <c r="D10">
-        <v>-25.399999999999977</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>4.4166666666666652</v>
-      </c>
-      <c r="C11" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B11, 0)</f>
-        <v>26102</v>
-      </c>
-      <c r="D11">
-        <v>-23.800000000000011</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>4.4999999999999982</v>
-      </c>
-      <c r="C12" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B12, 0)</f>
-        <v>31623</v>
-      </c>
-      <c r="D12">
-        <v>-16.899999999999977</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <f>B12 + (1/12)</f>
-        <v>4.5833333333333313</v>
-      </c>
-      <c r="C13" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B13, 0)</f>
-        <v>38312</v>
-      </c>
-      <c r="D13">
-        <v>-14.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <f t="shared" ref="B14:B26" si="1">B13 + (1/12)</f>
-        <v>4.6666666666666643</v>
-      </c>
-      <c r="C14" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B14, 0)</f>
-        <v>46416</v>
-      </c>
-      <c r="D14">
-        <v>-12.600000000000023</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <f t="shared" si="1"/>
-        <v>4.7499999999999973</v>
-      </c>
-      <c r="C15" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B15, 0)</f>
-        <v>56235</v>
-      </c>
-      <c r="D15">
-        <v>-7.6000000000000227</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <f t="shared" si="1"/>
-        <v>4.8333333333333304</v>
-      </c>
-      <c r="C16" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B16, 0)</f>
-        <v>68130</v>
-      </c>
-      <c r="D16">
-        <v>-6.8999999999999773</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f t="shared" si="1"/>
-        <v>4.9166666666666634</v>
-      </c>
-      <c r="C17" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B17, 0)</f>
-        <v>82541</v>
-      </c>
-      <c r="D17">
-        <v>-6.5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f t="shared" si="1"/>
-        <v>4.9999999999999964</v>
-      </c>
-      <c r="C18" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B18, 0)</f>
-        <v>100000</v>
-      </c>
-      <c r="D18">
-        <v>-3.8999999999999773</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <f t="shared" si="1"/>
-        <v>5.0833333333333295</v>
-      </c>
-      <c r="C19" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B19, 0)</f>
-        <v>121153</v>
-      </c>
-      <c r="D19">
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <f t="shared" si="1"/>
-        <v>5.1666666666666625</v>
-      </c>
-      <c r="C20" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B20, 0)</f>
-        <v>146780</v>
-      </c>
-      <c r="D20">
-        <v>-0.30000000000001137</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f t="shared" si="1"/>
-        <v>5.2499999999999956</v>
-      </c>
-      <c r="C21" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B21, 0)</f>
-        <v>177828</v>
-      </c>
-      <c r="D21">
-        <v>1.379</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <f t="shared" si="1"/>
-        <v>5.3333333333333286</v>
-      </c>
-      <c r="C22" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B22, 0)</f>
-        <v>215444</v>
-      </c>
-      <c r="D22">
-        <v>1.667</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <f t="shared" si="1"/>
-        <v>5.4166666666666616</v>
-      </c>
-      <c r="C23" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B23, 0)</f>
-        <v>261016</v>
-      </c>
-      <c r="D23">
-        <v>4.774</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <f t="shared" si="1"/>
-        <v>5.4999999999999947</v>
-      </c>
-      <c r="C24" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B24, 0)</f>
-        <v>316228</v>
-      </c>
-      <c r="D24">
-        <v>5.2949999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <f t="shared" si="1"/>
-        <v>5.5833333333333277</v>
-      </c>
-      <c r="C25" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B25, 0)</f>
-        <v>383119</v>
-      </c>
-      <c r="D25">
-        <v>7.0990000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <f t="shared" si="1"/>
-        <v>5.6666666666666607</v>
-      </c>
-      <c r="C26" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B26, 0)</f>
-        <v>464159</v>
-      </c>
-      <c r="D26">
-        <v>7.7619999999999996</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <f>B26 + (1/12)</f>
-        <v>5.7499999999999938</v>
-      </c>
-      <c r="C27" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B27, 0)</f>
-        <v>562342</v>
-      </c>
-      <c r="D27">
-        <v>11.51</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <f t="shared" ref="B28:B46" si="2">B27 + (1/12)</f>
-        <v>5.8333333333333268</v>
-      </c>
-      <c r="C28" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B28, 0)</f>
-        <v>681293</v>
-      </c>
-      <c r="D28">
-        <v>16.52</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <f t="shared" si="2"/>
-        <v>5.9166666666666599</v>
-      </c>
-      <c r="C29" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B29, 0)</f>
-        <v>825405</v>
-      </c>
-      <c r="D29">
-        <v>18.54</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <f t="shared" si="2"/>
-        <v>5.9999999999999929</v>
-      </c>
-      <c r="C30" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B30, 0)</f>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <f t="shared" ref="B6:B69" si="0">B5+250000</f>
+        <v>250000</v>
+      </c>
+      <c r="C6">
+        <v>3.6960000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <f t="shared" si="0"/>
+        <v>500000</v>
+      </c>
+      <c r="C7">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <f t="shared" si="0"/>
+        <v>750000</v>
+      </c>
+      <c r="C8">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="D30">
-        <v>20.64</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <f t="shared" si="2"/>
-        <v>6.0833333333333259</v>
-      </c>
-      <c r="C31" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B31, 0)</f>
-        <v>1211528</v>
-      </c>
-      <c r="D31">
-        <v>27.16</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <f t="shared" si="2"/>
-        <v>6.166666666666659</v>
-      </c>
-      <c r="C32" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B32, 0)</f>
-        <v>1467800</v>
-      </c>
-      <c r="D32">
-        <v>32.99</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <f t="shared" si="2"/>
-        <v>6.249999999999992</v>
-      </c>
-      <c r="C33" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B33, 0)</f>
-        <v>1778280</v>
-      </c>
-      <c r="D33">
-        <v>39.97</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <f t="shared" si="2"/>
-        <v>6.333333333333325</v>
-      </c>
-      <c r="C34" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B34, 0)</f>
-        <v>2154435</v>
-      </c>
-      <c r="D34">
-        <v>47.71</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <f t="shared" si="2"/>
-        <v>6.4166666666666581</v>
-      </c>
-      <c r="C35" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B35, 0)</f>
-        <v>2610158</v>
-      </c>
-      <c r="D35">
-        <v>55.07</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <f t="shared" si="2"/>
-        <v>6.4999999999999911</v>
-      </c>
-      <c r="C36" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B36, 0)</f>
-        <v>3162278</v>
-      </c>
-      <c r="D36">
-        <v>67.75</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <f t="shared" si="2"/>
-        <v>6.5833333333333242</v>
-      </c>
-      <c r="C37" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B37, 0)</f>
-        <v>3831187</v>
-      </c>
-      <c r="D37">
-        <v>79.959999999999994</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <f t="shared" si="2"/>
-        <v>6.6666666666666572</v>
-      </c>
-      <c r="C38" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B38, 0)</f>
-        <v>4641589</v>
-      </c>
-      <c r="D38">
-        <v>93.81</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <f t="shared" si="2"/>
-        <v>6.7499999999999902</v>
-      </c>
-      <c r="C39" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B39, 0)</f>
-        <v>5623414</v>
-      </c>
-      <c r="D39">
-        <v>108.5</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <f t="shared" si="2"/>
-        <v>6.8333333333333233</v>
-      </c>
-      <c r="C40" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B40, 0)</f>
-        <v>6812921</v>
-      </c>
-      <c r="D40">
-        <v>129.69999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <f t="shared" si="2"/>
-        <v>6.9166666666666563</v>
-      </c>
-      <c r="C41" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B41, 0)</f>
-        <v>8254042</v>
-      </c>
-      <c r="D41">
-        <v>158.19999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <f t="shared" si="2"/>
-        <v>6.9999999999999893</v>
-      </c>
-      <c r="C42" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B42, 0)</f>
+      <c r="C9">
+        <v>23.31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <f t="shared" si="0"/>
+        <v>1250000</v>
+      </c>
+      <c r="C10">
+        <v>25.99</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <f t="shared" si="0"/>
+        <v>1500000</v>
+      </c>
+      <c r="C11">
+        <v>33.619999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
+        <f t="shared" si="0"/>
+        <v>1750000</v>
+      </c>
+      <c r="C12">
+        <v>35.950000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+      <c r="C13">
+        <v>38.96</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
+        <f t="shared" si="0"/>
+        <v>2250000</v>
+      </c>
+      <c r="C14">
+        <v>46.43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
+        <f t="shared" si="0"/>
+        <v>2500000</v>
+      </c>
+      <c r="C15">
+        <v>51.31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <f t="shared" si="0"/>
+        <v>2750000</v>
+      </c>
+      <c r="C16">
+        <v>55.13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
+        <f t="shared" si="0"/>
+        <v>3000000</v>
+      </c>
+      <c r="C17">
+        <v>59.42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
+        <f t="shared" si="0"/>
+        <v>3250000</v>
+      </c>
+      <c r="C18">
+        <v>65.06</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
+        <f t="shared" si="0"/>
+        <v>3500000</v>
+      </c>
+      <c r="C19">
+        <v>67.430000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <f t="shared" si="0"/>
+        <v>3750000</v>
+      </c>
+      <c r="C20">
+        <v>73.680000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="7">
+        <f t="shared" si="0"/>
+        <v>4000000</v>
+      </c>
+      <c r="C21">
+        <v>73.81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="7">
+        <f t="shared" si="0"/>
+        <v>4250000</v>
+      </c>
+      <c r="C22">
+        <v>81.44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="7">
+        <f t="shared" si="0"/>
+        <v>4500000</v>
+      </c>
+      <c r="C23">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="7">
+        <f t="shared" si="0"/>
+        <v>4750000</v>
+      </c>
+      <c r="C24">
+        <v>89.18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
+        <f t="shared" si="0"/>
+        <v>5000000</v>
+      </c>
+      <c r="C25">
+        <v>89.44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <f t="shared" si="0"/>
+        <v>5250000</v>
+      </c>
+      <c r="C26">
+        <v>95.54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
+        <f t="shared" si="0"/>
+        <v>5500000</v>
+      </c>
+      <c r="C27">
+        <v>99.01</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
+        <f t="shared" si="0"/>
+        <v>5750000</v>
+      </c>
+      <c r="C28">
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
+        <f t="shared" si="0"/>
+        <v>6000000</v>
+      </c>
+      <c r="C29">
+        <v>109.2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
+        <f t="shared" si="0"/>
+        <v>6250000</v>
+      </c>
+      <c r="C30">
+        <v>113.7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="7">
+        <f t="shared" si="0"/>
+        <v>6500000</v>
+      </c>
+      <c r="C31">
+        <v>114.2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="7">
+        <f t="shared" si="0"/>
+        <v>6750000</v>
+      </c>
+      <c r="C32">
+        <v>121.1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="7">
+        <f t="shared" si="0"/>
+        <v>7000000</v>
+      </c>
+      <c r="C33">
+        <v>125.4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="7">
+        <f t="shared" si="0"/>
+        <v>7250000</v>
+      </c>
+      <c r="C34">
+        <v>130.9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="7">
+        <f t="shared" si="0"/>
+        <v>7500000</v>
+      </c>
+      <c r="C35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="7">
+        <f t="shared" si="0"/>
+        <v>7750000</v>
+      </c>
+      <c r="C36">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="7">
+        <f t="shared" si="0"/>
+        <v>8000000</v>
+      </c>
+      <c r="C37">
+        <v>146.6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="7">
+        <f t="shared" si="0"/>
+        <v>8250000</v>
+      </c>
+      <c r="C38">
+        <v>153.6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="7">
+        <f t="shared" si="0"/>
+        <v>8500000</v>
+      </c>
+      <c r="C39">
+        <v>162.4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="7">
+        <f t="shared" si="0"/>
+        <v>8750000</v>
+      </c>
+      <c r="C40">
+        <v>165.5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="7">
+        <f t="shared" si="0"/>
+        <v>9000000</v>
+      </c>
+      <c r="C41">
+        <v>172.9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="7">
+        <f t="shared" si="0"/>
+        <v>9250000</v>
+      </c>
+      <c r="C42">
+        <v>176.7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="7">
+        <f t="shared" si="0"/>
+        <v>9500000</v>
+      </c>
+      <c r="C43">
+        <v>188.8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="7">
+        <f t="shared" si="0"/>
+        <v>9750000</v>
+      </c>
+      <c r="C44">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="7">
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
-      <c r="D42">
-        <v>206.8</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <f t="shared" si="2"/>
-        <v>7.0833333333333224</v>
-      </c>
-      <c r="C43" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B43, 0)</f>
-        <v>12115277</v>
-      </c>
-      <c r="D43">
-        <v>258.10000000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <f t="shared" si="2"/>
-        <v>7.1666666666666554</v>
-      </c>
-      <c r="C44" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B44, 0)</f>
-        <v>14677993</v>
-      </c>
-      <c r="D44">
-        <v>24.48</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <f t="shared" si="2"/>
-        <v>7.2499999999999885</v>
-      </c>
-      <c r="C45" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B45, 0)</f>
-        <v>17782795</v>
-      </c>
-      <c r="D45" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <f t="shared" si="2"/>
-        <v>7.3333333333333215</v>
-      </c>
-      <c r="C46" s="7">
-        <f xml:space="preserve"> ROUNDUP(10 ^ B46, 0)</f>
-        <v>21544347</v>
-      </c>
-      <c r="D46" t="s">
-        <v>16</v>
+      <c r="C45">
+        <v>199.7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="7">
+        <f t="shared" si="0"/>
+        <v>10250000</v>
+      </c>
+      <c r="C46">
+        <v>205.6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="7">
+        <f t="shared" si="0"/>
+        <v>10500000</v>
+      </c>
+      <c r="C47">
+        <v>214.8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="7">
+        <f t="shared" si="0"/>
+        <v>10750000</v>
+      </c>
+      <c r="C48">
+        <v>218.7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="7">
+        <f t="shared" si="0"/>
+        <v>11000000</v>
+      </c>
+      <c r="C49">
+        <v>226.2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="7">
+        <f t="shared" si="0"/>
+        <v>11250000</v>
+      </c>
+      <c r="C50">
+        <v>233.7</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="7">
+        <f t="shared" si="0"/>
+        <v>11500000</v>
+      </c>
+      <c r="C51">
+        <v>237.7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="7">
+        <f t="shared" si="0"/>
+        <v>11750000</v>
+      </c>
+      <c r="C52">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="7">
+        <f t="shared" si="0"/>
+        <v>12000000</v>
+      </c>
+      <c r="C53">
+        <v>249.9</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="7">
+        <f t="shared" si="0"/>
+        <v>12250000</v>
+      </c>
+      <c r="C54">
+        <v>254.2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="7">
+        <f t="shared" si="0"/>
+        <v>12500000</v>
+      </c>
+      <c r="C55">
+        <v>261.8</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="7">
+        <f t="shared" si="0"/>
+        <v>12750000</v>
+      </c>
+      <c r="C56">
+        <v>263.89999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="7">
+        <f t="shared" si="0"/>
+        <v>13000000</v>
+      </c>
+      <c r="C57">
+        <v>269.3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="7">
+        <f t="shared" si="0"/>
+        <v>13250000</v>
+      </c>
+      <c r="C58">
+        <v>281.3</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="7">
+        <f t="shared" si="0"/>
+        <v>13500000</v>
+      </c>
+      <c r="C59">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="7">
+        <f t="shared" si="0"/>
+        <v>13750000</v>
+      </c>
+      <c r="C60">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="7">
+        <f t="shared" si="0"/>
+        <v>14000000</v>
+      </c>
+      <c r="C61">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="7">
+        <f t="shared" si="0"/>
+        <v>14250000</v>
+      </c>
+      <c r="C62">
+        <v>357.3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="7">
+        <f t="shared" si="0"/>
+        <v>14500000</v>
+      </c>
+      <c r="C63">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="7">
+        <f t="shared" si="0"/>
+        <v>14750000</v>
+      </c>
+      <c r="C64">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="7">
+        <f t="shared" si="0"/>
+        <v>15000000</v>
+      </c>
+      <c r="C65">
+        <v>48.96</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="7">
+        <f t="shared" si="0"/>
+        <v>15250000</v>
+      </c>
+      <c r="C66">
+        <v>60.41</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="7">
+        <f t="shared" si="0"/>
+        <v>15500000</v>
+      </c>
+      <c r="C67">
+        <v>69.930000000000007</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="7">
+        <f t="shared" si="0"/>
+        <v>15750000</v>
+      </c>
+      <c r="C68">
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="7">
+        <f t="shared" si="0"/>
+        <v>16000000</v>
+      </c>
+      <c r="C69">
+        <v>81.569999999999993</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Updated documentation file with additional graph
</commit_message>
<xml_diff>
--- a/Documentation/DdD Gain and filter calculations.xlsx
+++ b/Documentation/DdD Gain and filter calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simon\Documents\GitHub\DomesdayDuplicator\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7089AA06-0089-4023-897F-9DBED4C9683F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E513D039-6B77-40C4-8252-966C54EF0795}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="38400" windowHeight="17610" activeTab="1" xr2:uid="{6586ADF8-B05F-4BD6-A150-BEC042DE64BB}"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="38400" windowHeight="17610" activeTab="1" xr2:uid="{6586ADF8-B05F-4BD6-A150-BEC042DE64BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequency Response" sheetId="3" r:id="rId1"/>
@@ -1810,6 +1810,7 @@
         <c:axId val="993010496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="16000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1827,6 +1828,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frequency (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1891,6 +1947,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Phase (degrees)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7727,7 +7838,7 @@
   <dimension ref="B4:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>